<commit_message>
Use new datasets from v8.2
- Adapt SSFA_1_Import.Rmd: edit "Names" in the ConfoMap datasets, remove upper-case letters in treatment names (except first letter), re-order cleaning procedures for plotting.
- Rename RStudioVersion.txt to SSFA_0_RStudioVersion.txt
- Adapt SSFA_Plots.Rmd (WIP): position all boxes at the correct place even when only one box (NewEpLsar), standarize width of boxes in sheep and guinea pig datasets, move legend to bottom without title, adjust printing size to 190x240 mm.
</commit_message>
<xml_diff>
--- a/R_analysis/derived_data/SSFA_all_data.xlsx
+++ b/R_analysis/derived_data/SSFA_all_data.xlsx
@@ -63,7 +63,7 @@
     <t xml:space="preserve">ConfoMap</t>
   </si>
   <si>
-    <t xml:space="preserve">Dry Lucerne</t>
+    <t xml:space="preserve">Dry lucerne</t>
   </si>
   <si>
     <t xml:space="preserve">Toothfrax</t>
@@ -141,7 +141,7 @@
     <t xml:space="preserve">capor_2CC5B1_txP4_#1_1_100xL_1</t>
   </si>
   <si>
-    <t xml:space="preserve">Dry Grass</t>
+    <t xml:space="preserve">Dry grass</t>
   </si>
   <si>
     <t xml:space="preserve">capor_2CC5B1_txP4_#1_1_100xL_2</t>
@@ -210,7 +210,7 @@
     <t xml:space="preserve">capor_2CC6B1_txP4_#1_1_100xL_1</t>
   </si>
   <si>
-    <t xml:space="preserve">Dry Bamboo</t>
+    <t xml:space="preserve">Dry bamboo</t>
   </si>
   <si>
     <t xml:space="preserve">capor_2CC6B1_txP4_#1_1_100xL_2</t>
@@ -432,7 +432,7 @@
     <t xml:space="preserve">L6-Ovis-10106-lm2sin-a</t>
   </si>
   <si>
-    <t xml:space="preserve">Clover+Dust</t>
+    <t xml:space="preserve">Clover+dust</t>
   </si>
   <si>
     <t xml:space="preserve">L6-Ovis-11707-lm2sin-a</t>
@@ -498,7 +498,7 @@
     <t xml:space="preserve">L8-Ovis-00234-lm2sin-a</t>
   </si>
   <si>
-    <t xml:space="preserve">Grass+Dust</t>
+    <t xml:space="preserve">Grass+dust</t>
   </si>
   <si>
     <t xml:space="preserve">L8-Ovis-08043-lm2sin-a</t>
@@ -932,25 +932,25 @@
       <c r="E2"/>
       <c r="F2"/>
       <c r="G2" t="n">
-        <v>0.001960011</v>
+        <v>0.002067360545</v>
       </c>
       <c r="H2" t="n">
-        <v>0.998370268</v>
+        <v>0.9980104634</v>
       </c>
       <c r="I2" t="n">
-        <v>14.29322597</v>
+        <v>10.78159498</v>
       </c>
       <c r="J2" t="n">
-        <v>0.415393778</v>
+        <v>0.4484673392</v>
       </c>
       <c r="K2" t="n">
-        <v>0.164461792</v>
+        <v>0.1806015748</v>
       </c>
       <c r="L2" t="n">
-        <v>0.368123892</v>
+        <v>0.3645721331</v>
       </c>
       <c r="M2" t="n">
-        <v>0.01842431</v>
+        <v>0.01846373024</v>
       </c>
     </row>
     <row r="3">
@@ -1004,25 +1004,25 @@
       <c r="E4"/>
       <c r="F4"/>
       <c r="G4" t="n">
-        <v>0.003662312</v>
+        <v>0.003812139616</v>
       </c>
       <c r="H4" t="n">
-        <v>0.999112342</v>
+        <v>0.9984253117</v>
       </c>
       <c r="I4" t="n">
-        <v>12.90554867</v>
+        <v>10.03406338</v>
       </c>
       <c r="J4" t="n">
-        <v>0.440817926</v>
+        <v>0.5913959046</v>
       </c>
       <c r="K4" t="n">
-        <v>0.171361361</v>
+        <v>0.1895997081</v>
       </c>
       <c r="L4" t="n">
-        <v>0.417234053</v>
+        <v>0.4065172016</v>
       </c>
       <c r="M4" t="n">
-        <v>0.018888664</v>
+        <v>0.01896205204</v>
       </c>
     </row>
     <row r="5">
@@ -1076,25 +1076,25 @@
       <c r="E6"/>
       <c r="F6"/>
       <c r="G6" t="n">
-        <v>0.003140386</v>
+        <v>0.0032705209</v>
       </c>
       <c r="H6" t="n">
-        <v>0.998934822</v>
+        <v>0.9984925822</v>
       </c>
       <c r="I6" t="n">
-        <v>13.66607046</v>
+        <v>10.49784966</v>
       </c>
       <c r="J6" t="n">
-        <v>0.440817926</v>
+        <v>0.5913959046</v>
       </c>
       <c r="K6" t="n">
-        <v>0.130528691</v>
+        <v>0.1137788648</v>
       </c>
       <c r="L6" t="n">
-        <v>0.352168709</v>
+        <v>0.3633146615</v>
       </c>
       <c r="M6" t="n">
-        <v>0.018703144</v>
+        <v>0.01875636554</v>
       </c>
     </row>
     <row r="7">
@@ -1148,25 +1148,25 @@
       <c r="E8"/>
       <c r="F8"/>
       <c r="G8" t="n">
-        <v>0.002768482</v>
+        <v>0.002905051355</v>
       </c>
       <c r="H8" t="n">
-        <v>0.998438105</v>
+        <v>0.9983854869</v>
       </c>
       <c r="I8" t="n">
-        <v>11.69780996</v>
+        <v>9.213448104</v>
       </c>
       <c r="J8" t="n">
-        <v>0.496429712</v>
+        <v>0.5913959046</v>
       </c>
       <c r="K8" t="n">
-        <v>0.428999312</v>
+        <v>0.4021779541</v>
       </c>
       <c r="L8" t="n">
-        <v>0.618111286</v>
+        <v>0.5843529378</v>
       </c>
       <c r="M8" t="n">
-        <v>0.01874769</v>
+        <v>0.01880623489</v>
       </c>
     </row>
     <row r="9">
@@ -1220,25 +1220,25 @@
       <c r="E10"/>
       <c r="F10"/>
       <c r="G10" t="n">
-        <v>0.001196562</v>
+        <v>0.001256082569</v>
       </c>
       <c r="H10" t="n">
-        <v>0.998787959</v>
+        <v>0.9981482811</v>
       </c>
       <c r="I10" t="n">
-        <v>13.96724829</v>
+        <v>10.70664486</v>
       </c>
       <c r="J10" t="n">
-        <v>0.415393778</v>
+        <v>0.6605980842</v>
       </c>
       <c r="K10" t="n">
-        <v>0.120905484</v>
+        <v>0.0982992664</v>
       </c>
       <c r="L10" t="n">
-        <v>0.381337164</v>
+        <v>0.3639581152</v>
       </c>
       <c r="M10" t="n">
-        <v>0.018092915</v>
+        <v>0.01812418726</v>
       </c>
     </row>
     <row r="11">
@@ -1292,25 +1292,25 @@
       <c r="E12"/>
       <c r="F12"/>
       <c r="G12" t="n">
-        <v>0.002076586</v>
+        <v>0.00216625291</v>
       </c>
       <c r="H12" t="n">
-        <v>0.999087134</v>
+        <v>0.9984843969</v>
       </c>
       <c r="I12" t="n">
-        <v>14.30217635</v>
+        <v>11.08783302</v>
       </c>
       <c r="J12" t="n">
-        <v>0.440817926</v>
+        <v>0.5913959046</v>
       </c>
       <c r="K12" t="n">
-        <v>0.171286315</v>
+        <v>0.1839794215</v>
       </c>
       <c r="L12" t="n">
-        <v>0.402287477</v>
+        <v>0.4416767432</v>
       </c>
       <c r="M12" t="n">
-        <v>0.018557445</v>
+        <v>0.01859686825</v>
       </c>
     </row>
     <row r="13">
@@ -1364,25 +1364,25 @@
       <c r="E14"/>
       <c r="F14"/>
       <c r="G14" t="n">
-        <v>0.002243407</v>
+        <v>0.002329122824</v>
       </c>
       <c r="H14" t="n">
-        <v>0.998884668</v>
+        <v>0.9980501357</v>
       </c>
       <c r="I14" t="n">
-        <v>13.40110065</v>
+        <v>10.34937863</v>
       </c>
       <c r="J14" t="n">
-        <v>0.467798158</v>
+        <v>0.5913959046</v>
       </c>
       <c r="K14" t="n">
-        <v>0.194389173</v>
+        <v>0.2014663409</v>
       </c>
       <c r="L14" t="n">
-        <v>0.390500798</v>
+        <v>0.3738601095</v>
       </c>
       <c r="M14" t="n">
-        <v>0.018099969</v>
+        <v>0.01812683641</v>
       </c>
     </row>
     <row r="15">
@@ -1436,25 +1436,25 @@
       <c r="E16"/>
       <c r="F16"/>
       <c r="G16" t="n">
-        <v>0.002798591</v>
+        <v>0.002979540156</v>
       </c>
       <c r="H16" t="n">
-        <v>0.999103476</v>
+        <v>0.9986605569</v>
       </c>
       <c r="I16" t="n">
-        <v>14.76705164</v>
+        <v>11.2648305</v>
       </c>
       <c r="J16" t="n">
-        <v>0.415393778</v>
+        <v>0.5913959046</v>
       </c>
       <c r="K16" t="n">
-        <v>0.141126487</v>
+        <v>0.1267008418</v>
       </c>
       <c r="L16" t="n">
-        <v>0.376485825</v>
+        <v>0.3744819759</v>
       </c>
       <c r="M16" t="n">
-        <v>0.018786464</v>
+        <v>0.01885447729</v>
       </c>
     </row>
     <row r="17">
@@ -1508,25 +1508,25 @@
       <c r="E18"/>
       <c r="F18"/>
       <c r="G18" t="n">
-        <v>0.002215594</v>
+        <v>0.002359142165</v>
       </c>
       <c r="H18" t="n">
-        <v>0.998493777</v>
+        <v>0.9988543057</v>
       </c>
       <c r="I18" t="n">
-        <v>13.92211229</v>
+        <v>10.34681011</v>
       </c>
       <c r="J18" t="n">
-        <v>0.36885992</v>
+        <v>0.4739803294</v>
       </c>
       <c r="K18" t="n">
-        <v>0.276417135</v>
+        <v>0.2753693702</v>
       </c>
       <c r="L18" t="n">
-        <v>0.371585356</v>
+        <v>0.368393954</v>
       </c>
       <c r="M18" t="n">
-        <v>0.018206709</v>
+        <v>0.01825467099</v>
       </c>
     </row>
     <row r="19">
@@ -1580,25 +1580,25 @@
       <c r="E20"/>
       <c r="F20"/>
       <c r="G20" t="n">
-        <v>0.001822602</v>
+        <v>0.001957674067</v>
       </c>
       <c r="H20" t="n">
-        <v>0.998902359</v>
+        <v>0.9985564736</v>
       </c>
       <c r="I20" t="n">
-        <v>16.68481104</v>
+        <v>11.7449645</v>
       </c>
       <c r="J20" t="n">
-        <v>0.290846892</v>
+        <v>0.4014873099</v>
       </c>
       <c r="K20" t="n">
-        <v>0.188809059</v>
+        <v>0.1972258018</v>
       </c>
       <c r="L20" t="n">
-        <v>0.309204915</v>
+        <v>0.3176914814</v>
       </c>
       <c r="M20" t="n">
-        <v>0.018396108</v>
+        <v>0.01845889031</v>
       </c>
     </row>
     <row r="21">
@@ -1652,25 +1652,25 @@
       <c r="E22"/>
       <c r="F22"/>
       <c r="G22" t="n">
-        <v>0.001195386</v>
+        <v>0.001262324071</v>
       </c>
       <c r="H22" t="n">
-        <v>0.998836037</v>
+        <v>0.9989192509</v>
       </c>
       <c r="I22" t="n">
-        <v>13.97496596</v>
+        <v>9.995706299</v>
       </c>
       <c r="J22" t="n">
-        <v>0.347585945</v>
+        <v>0.5595627735</v>
       </c>
       <c r="K22" t="n">
-        <v>0.142846338</v>
+        <v>0.1427693559</v>
       </c>
       <c r="L22" t="n">
-        <v>0.35436911</v>
+        <v>0.3554464415</v>
       </c>
       <c r="M22" t="n">
-        <v>0.01808377</v>
+        <v>0.01811654818</v>
       </c>
     </row>
     <row r="23">
@@ -1724,25 +1724,25 @@
       <c r="E24"/>
       <c r="F24"/>
       <c r="G24" t="n">
-        <v>0.001549638</v>
+        <v>0.001630660524</v>
       </c>
       <c r="H24" t="n">
-        <v>0.998881244</v>
+        <v>0.9985356569</v>
       </c>
       <c r="I24" t="n">
-        <v>13.05343267</v>
+        <v>9.336848568</v>
       </c>
       <c r="J24" t="n">
-        <v>0.327538946</v>
+        <v>0.4484673392</v>
       </c>
       <c r="K24" t="n">
-        <v>0.162233111</v>
+        <v>0.1907005473</v>
       </c>
       <c r="L24" t="n">
-        <v>0.374577162</v>
+        <v>0.3631057954</v>
       </c>
       <c r="M24" t="n">
-        <v>0.018262853</v>
+        <v>0.01830189158</v>
       </c>
     </row>
     <row r="25">
@@ -1796,25 +1796,25 @@
       <c r="E26"/>
       <c r="F26"/>
       <c r="G26" t="n">
-        <v>0.003795656</v>
+        <v>0.003929549878</v>
       </c>
       <c r="H26" t="n">
-        <v>0.997779083</v>
+        <v>0.998252843</v>
       </c>
       <c r="I26" t="n">
-        <v>9.198882044</v>
+        <v>6.466741226</v>
       </c>
       <c r="J26" t="n">
-        <v>0.229333441</v>
+        <v>0.5294431279</v>
       </c>
       <c r="K26" t="n">
-        <v>0.359553297</v>
+        <v>0.3714519093</v>
       </c>
       <c r="L26" t="n">
-        <v>0.612984794</v>
+        <v>0.6287885129</v>
       </c>
       <c r="M26" t="n">
-        <v>0.019249182</v>
+        <v>0.01930272211</v>
       </c>
     </row>
     <row r="27">
@@ -1868,25 +1868,25 @@
       <c r="E28"/>
       <c r="F28"/>
       <c r="G28" t="n">
-        <v>0.003107149</v>
+        <v>0.003268662423</v>
       </c>
       <c r="H28" t="n">
-        <v>0.998459016</v>
+        <v>0.9984441562</v>
       </c>
       <c r="I28" t="n">
-        <v>8.951343639</v>
+        <v>5.524081785</v>
       </c>
       <c r="J28" t="n">
-        <v>0.216106648</v>
+        <v>0.3400817502</v>
       </c>
       <c r="K28" t="n">
-        <v>0.216203797</v>
+        <v>0.218989173</v>
       </c>
       <c r="L28" t="n">
-        <v>0.465230414</v>
+        <v>0.4534555845</v>
       </c>
       <c r="M28" t="n">
-        <v>0.018844878</v>
+        <v>0.01891031759</v>
       </c>
     </row>
     <row r="29">
@@ -1940,25 +1940,25 @@
       <c r="E30"/>
       <c r="F30"/>
       <c r="G30" t="n">
-        <v>0.003620257</v>
+        <v>0.003796207059</v>
       </c>
       <c r="H30" t="n">
-        <v>0.998451979</v>
+        <v>0.9984525507</v>
       </c>
       <c r="I30" t="n">
-        <v>12.69495698</v>
+        <v>8.94383515</v>
       </c>
       <c r="J30" t="n">
-        <v>0.290846892</v>
+        <v>0.4014873099</v>
       </c>
       <c r="K30" t="n">
-        <v>0.329425381</v>
+        <v>0.3553912332</v>
       </c>
       <c r="L30" t="n">
-        <v>0.506567784</v>
+        <v>0.4932898395</v>
       </c>
       <c r="M30" t="n">
-        <v>0.018733928</v>
+        <v>0.01880308052</v>
       </c>
     </row>
     <row r="31">
@@ -2012,25 +2012,25 @@
       <c r="E32"/>
       <c r="F32"/>
       <c r="G32" t="n">
-        <v>0.002175306</v>
+        <v>0.002354811272</v>
       </c>
       <c r="H32" t="n">
-        <v>0.998600483</v>
+        <v>0.9981375962</v>
       </c>
       <c r="I32" t="n">
-        <v>14.54498781</v>
+        <v>11.54435729</v>
       </c>
       <c r="J32" t="n">
-        <v>0.36885992</v>
+        <v>0.5595627735</v>
       </c>
       <c r="K32" t="n">
-        <v>0.317777021</v>
+        <v>0.3440217544</v>
       </c>
       <c r="L32" t="n">
-        <v>0.855690281</v>
+        <v>0.9249893402</v>
       </c>
       <c r="M32" t="n">
-        <v>0.018357147</v>
+        <v>0.01839624876</v>
       </c>
     </row>
     <row r="33">
@@ -2084,25 +2084,25 @@
       <c r="E34"/>
       <c r="F34"/>
       <c r="G34" t="n">
-        <v>0.001591789</v>
+        <v>0.001663628121</v>
       </c>
       <c r="H34" t="n">
-        <v>0.997532386</v>
+        <v>0.9987746354</v>
       </c>
       <c r="I34" t="n">
-        <v>9.82824833</v>
+        <v>7.055495681</v>
       </c>
       <c r="J34" t="n">
-        <v>0.308648157</v>
+        <v>0.62504</v>
       </c>
       <c r="K34" t="n">
-        <v>0.266301696</v>
+        <v>0.3060963179</v>
       </c>
       <c r="L34" t="n">
-        <v>0.43967751</v>
+        <v>0.5001416965</v>
       </c>
       <c r="M34" t="n">
-        <v>0.018264982</v>
+        <v>0.01829563078</v>
       </c>
     </row>
     <row r="35">
@@ -2156,25 +2156,25 @@
       <c r="E36"/>
       <c r="F36"/>
       <c r="G36" t="n">
-        <v>0.002970947</v>
+        <v>0.003115539578</v>
       </c>
       <c r="H36" t="n">
-        <v>0.999056544</v>
+        <v>0.9982992722</v>
       </c>
       <c r="I36" t="n">
-        <v>19.46945807</v>
+        <v>15.45003357</v>
       </c>
       <c r="J36" t="n">
-        <v>0.391435966</v>
+        <v>0.4014873099</v>
       </c>
       <c r="K36" t="n">
-        <v>0.174551939</v>
+        <v>0.1727344328</v>
       </c>
       <c r="L36" t="n">
-        <v>0.357505425</v>
+        <v>0.3439220321</v>
       </c>
       <c r="M36" t="n">
-        <v>0.018811522</v>
+        <v>0.01887225737</v>
       </c>
     </row>
     <row r="37">
@@ -2228,25 +2228,25 @@
       <c r="E38"/>
       <c r="F38"/>
       <c r="G38" t="n">
-        <v>0.001601512</v>
+        <v>0.001705398015</v>
       </c>
       <c r="H38" t="n">
-        <v>0.99809759</v>
+        <v>0.9982986958</v>
       </c>
       <c r="I38" t="n">
-        <v>12.34565738</v>
+        <v>8.942898683</v>
       </c>
       <c r="J38" t="n">
-        <v>0.347585945</v>
+        <v>0.4014873099</v>
       </c>
       <c r="K38" t="n">
-        <v>0.165888947</v>
+        <v>0.1679042444</v>
       </c>
       <c r="L38" t="n">
-        <v>0.327854103</v>
+        <v>0.3339867358</v>
       </c>
       <c r="M38" t="n">
-        <v>0.018105923</v>
+        <v>0.01814504674</v>
       </c>
     </row>
     <row r="39">
@@ -2300,25 +2300,25 @@
       <c r="E40"/>
       <c r="F40"/>
       <c r="G40" t="n">
-        <v>0.002125456</v>
+        <v>0.002253830386</v>
       </c>
       <c r="H40" t="n">
-        <v>0.998572862</v>
+        <v>0.99831174</v>
       </c>
       <c r="I40" t="n">
-        <v>11.85442574</v>
+        <v>7.495995542</v>
       </c>
       <c r="J40" t="n">
-        <v>0.216106648</v>
+        <v>0.3400817502</v>
       </c>
       <c r="K40" t="n">
-        <v>0.322341529</v>
+        <v>0.3044743911</v>
       </c>
       <c r="L40" t="n">
-        <v>0.540434123</v>
+        <v>0.5371772648</v>
       </c>
       <c r="M40" t="n">
-        <v>0.018518889</v>
+        <v>0.01857516206</v>
       </c>
     </row>
     <row r="41">
@@ -2372,25 +2372,25 @@
       <c r="E42"/>
       <c r="F42"/>
       <c r="G42" t="n">
-        <v>0.004348138</v>
+        <v>0.004547933282</v>
       </c>
       <c r="H42" t="n">
-        <v>0.998926142</v>
+        <v>0.998428357</v>
       </c>
       <c r="I42" t="n">
-        <v>19.57223708</v>
+        <v>15.72230321</v>
       </c>
       <c r="J42" t="n">
-        <v>0.496429712</v>
+        <v>0.62504</v>
       </c>
       <c r="K42" t="n">
-        <v>0.272055042</v>
+        <v>0.2961005508</v>
       </c>
       <c r="L42" t="n">
-        <v>0.4447932</v>
+        <v>0.4392845422</v>
       </c>
       <c r="M42" t="n">
-        <v>0.019016673</v>
+        <v>0.01908976198</v>
       </c>
     </row>
     <row r="43">
@@ -2444,25 +2444,25 @@
       <c r="E44"/>
       <c r="F44"/>
       <c r="G44" t="n">
-        <v>0.002850841</v>
+        <v>0.002938725426</v>
       </c>
       <c r="H44" t="n">
-        <v>0.997779126</v>
+        <v>0.9979155975</v>
       </c>
       <c r="I44" t="n">
-        <v>10.58953187</v>
+        <v>7.907520979</v>
       </c>
       <c r="J44" t="n">
-        <v>0.36885992</v>
+        <v>0.62504</v>
       </c>
       <c r="K44" t="n">
-        <v>0.355257269</v>
+        <v>0.3604897494</v>
       </c>
       <c r="L44" t="n">
-        <v>0.44764112</v>
+        <v>0.4350251891</v>
       </c>
       <c r="M44" t="n">
-        <v>0.018068187</v>
+        <v>0.01811085623</v>
       </c>
     </row>
     <row r="45">
@@ -2516,25 +2516,25 @@
       <c r="E46"/>
       <c r="F46"/>
       <c r="G46" t="n">
-        <v>0.003797344</v>
+        <v>0.003969614705</v>
       </c>
       <c r="H46" t="n">
-        <v>0.998922708</v>
+        <v>0.9982339473</v>
       </c>
       <c r="I46" t="n">
-        <v>10.80422431</v>
+        <v>8.41067031</v>
       </c>
       <c r="J46" t="n">
-        <v>0.467798158</v>
+        <v>0.62504</v>
       </c>
       <c r="K46" t="n">
-        <v>0.390567081</v>
+        <v>0.3463455333</v>
       </c>
       <c r="L46" t="n">
-        <v>0.517974252</v>
+        <v>0.5005469836</v>
       </c>
       <c r="M46" t="n">
-        <v>0.018998086</v>
+        <v>0.01907269566</v>
       </c>
     </row>
     <row r="47">
@@ -2588,25 +2588,25 @@
       <c r="E48"/>
       <c r="F48"/>
       <c r="G48" t="n">
-        <v>0.003188218</v>
+        <v>0.003322627439</v>
       </c>
       <c r="H48" t="n">
-        <v>0.998977523</v>
+        <v>0.998245991</v>
       </c>
       <c r="I48" t="n">
-        <v>10.99011617</v>
+        <v>8.465339104</v>
       </c>
       <c r="J48" t="n">
-        <v>0.440817926</v>
+        <v>0.62504</v>
       </c>
       <c r="K48" t="n">
-        <v>0.261503983</v>
+        <v>0.2723396676</v>
       </c>
       <c r="L48" t="n">
-        <v>0.541313811</v>
+        <v>0.5133933412</v>
       </c>
       <c r="M48" t="n">
-        <v>0.018788637</v>
+        <v>0.01884591831</v>
       </c>
     </row>
     <row r="49">
@@ -2660,25 +2660,25 @@
       <c r="E50"/>
       <c r="F50"/>
       <c r="G50" t="n">
-        <v>0.002170894</v>
+        <v>0.002267447402</v>
       </c>
       <c r="H50" t="n">
-        <v>0.998886935</v>
+        <v>0.9986023958</v>
       </c>
       <c r="I50" t="n">
-        <v>14.47783465</v>
+        <v>11.70351676</v>
       </c>
       <c r="J50" t="n">
-        <v>0.559057254</v>
+        <v>0.6981790427</v>
       </c>
       <c r="K50" t="n">
-        <v>0.160252423</v>
+        <v>0.1612149107</v>
       </c>
       <c r="L50" t="n">
-        <v>0.334040064</v>
+        <v>0.360339211</v>
       </c>
       <c r="M50" t="n">
-        <v>0.018309949</v>
+        <v>0.01835327857</v>
       </c>
     </row>
     <row r="51">
@@ -2732,25 +2732,25 @@
       <c r="E52"/>
       <c r="F52"/>
       <c r="G52" t="n">
-        <v>0.002185925</v>
+        <v>0.002315536851</v>
       </c>
       <c r="H52" t="n">
-        <v>0.998755441</v>
+        <v>0.9984121867</v>
       </c>
       <c r="I52" t="n">
-        <v>11.36441184</v>
+        <v>8.651749525</v>
       </c>
       <c r="J52" t="n">
-        <v>0.467798158</v>
+        <v>0.5913959046</v>
       </c>
       <c r="K52" t="n">
-        <v>0.453796861</v>
+        <v>0.397064544</v>
       </c>
       <c r="L52" t="n">
-        <v>0.508169749</v>
+        <v>0.4682834602</v>
       </c>
       <c r="M52" t="n">
-        <v>0.017385439</v>
+        <v>0.01737486438</v>
       </c>
     </row>
     <row r="53">
@@ -2804,25 +2804,25 @@
       <c r="E54"/>
       <c r="F54"/>
       <c r="G54" t="n">
-        <v>0.002652807</v>
+        <v>0.002741027655</v>
       </c>
       <c r="H54" t="n">
-        <v>0.998841942</v>
+        <v>0.9981770193</v>
       </c>
       <c r="I54" t="n">
-        <v>20.76175031</v>
+        <v>17.3752942</v>
       </c>
       <c r="J54" t="n">
-        <v>0.62958563</v>
+        <v>0.6605980842</v>
       </c>
       <c r="K54" t="n">
-        <v>0.501616031</v>
+        <v>0.4849714377</v>
       </c>
       <c r="L54" t="n">
-        <v>0.475892986</v>
+        <v>0.4435263122</v>
       </c>
       <c r="M54" t="n">
-        <v>0.018138229</v>
+        <v>0.01817478153</v>
       </c>
     </row>
     <row r="55">
@@ -2876,25 +2876,25 @@
       <c r="E56"/>
       <c r="F56"/>
       <c r="G56" t="n">
-        <v>0.003228675</v>
+        <v>0.003375043862</v>
       </c>
       <c r="H56" t="n">
-        <v>0.999042079</v>
+        <v>0.9989523375</v>
       </c>
       <c r="I56" t="n">
-        <v>16.87545858</v>
+        <v>13.23971979</v>
       </c>
       <c r="J56" t="n">
-        <v>0.391435966</v>
+        <v>0.5595627735</v>
       </c>
       <c r="K56" t="n">
-        <v>0.167611762</v>
+        <v>0.1754716318</v>
       </c>
       <c r="L56" t="n">
-        <v>0.389406237</v>
+        <v>0.401973915</v>
       </c>
       <c r="M56" t="n">
-        <v>0.01900251</v>
+        <v>0.0190570765</v>
       </c>
     </row>
     <row r="57">
@@ -2948,25 +2948,25 @@
       <c r="E58"/>
       <c r="F58"/>
       <c r="G58" t="n">
-        <v>0.000998821</v>
+        <v>0.001068320011</v>
       </c>
       <c r="H58" t="n">
-        <v>0.998525009</v>
+        <v>0.9984505623</v>
       </c>
       <c r="I58" t="n">
-        <v>12.30119029</v>
+        <v>8.8637718</v>
       </c>
       <c r="J58" t="n">
-        <v>0.347585945</v>
+        <v>0.4243276394</v>
       </c>
       <c r="K58" t="n">
-        <v>0.187445128</v>
+        <v>0.1999493438</v>
       </c>
       <c r="L58" t="n">
-        <v>0.405302467</v>
+        <v>0.4329448827</v>
       </c>
       <c r="M58" t="n">
-        <v>0.017328018</v>
+        <v>0.01732131021</v>
       </c>
     </row>
     <row r="59">
@@ -3020,25 +3020,25 @@
       <c r="E60"/>
       <c r="F60"/>
       <c r="G60" t="n">
-        <v>0.001423758</v>
+        <v>0.001697884249</v>
       </c>
       <c r="H60" t="n">
-        <v>0.998262677</v>
+        <v>0.9983643454</v>
       </c>
       <c r="I60" t="n">
-        <v>12.51253614</v>
+        <v>9.255288307</v>
       </c>
       <c r="J60" t="n">
-        <v>0.36885992</v>
+        <v>0.5913959046</v>
       </c>
       <c r="K60" t="n">
-        <v>0.259315909</v>
+        <v>0.3242903422</v>
       </c>
       <c r="L60" t="n">
-        <v>0.411046973</v>
+        <v>0.4793412276</v>
       </c>
       <c r="M60" t="n">
-        <v>0.018032043</v>
+        <v>0.0181398183</v>
       </c>
     </row>
     <row r="61">
@@ -3092,25 +3092,25 @@
       <c r="E62"/>
       <c r="F62"/>
       <c r="G62" t="n">
-        <v>0.000533998</v>
+        <v>0.0005679653766</v>
       </c>
       <c r="H62" t="n">
-        <v>0.998737118</v>
+        <v>0.9979434565</v>
       </c>
       <c r="I62" t="n">
-        <v>19.8794206</v>
+        <v>15.59663467</v>
       </c>
       <c r="J62" t="n">
-        <v>0.440817926</v>
+        <v>0.5595627735</v>
       </c>
       <c r="K62" t="n">
-        <v>0.177831666</v>
+        <v>0.1745040884</v>
       </c>
       <c r="L62" t="n">
-        <v>0.277592374</v>
+        <v>0.267574094</v>
       </c>
       <c r="M62" t="n">
-        <v>0.017487828</v>
+        <v>0.01747712875</v>
       </c>
     </row>
     <row r="63">
@@ -3164,25 +3164,25 @@
       <c r="E64"/>
       <c r="F64"/>
       <c r="G64" t="n">
-        <v>0.00109822</v>
+        <v>0.001191898962</v>
       </c>
       <c r="H64" t="n">
-        <v>0.998321206</v>
+        <v>0.9979947225</v>
       </c>
       <c r="I64" t="n">
-        <v>11.46798993</v>
+        <v>8.196790974</v>
       </c>
       <c r="J64" t="n">
-        <v>0.347585963</v>
+        <v>0.4014873817</v>
       </c>
       <c r="K64" t="n">
-        <v>0.173338388</v>
+        <v>0.2140281067</v>
       </c>
       <c r="L64" t="n">
-        <v>0.42973279</v>
+        <v>0.4456738268</v>
       </c>
       <c r="M64" t="n">
-        <v>0.017288718</v>
+        <v>0.01727077648</v>
       </c>
     </row>
     <row r="65">
@@ -3236,25 +3236,25 @@
       <c r="E66"/>
       <c r="F66"/>
       <c r="G66" t="n">
-        <v>0.000321969</v>
+        <v>0.0003473793101</v>
       </c>
       <c r="H66" t="n">
-        <v>0.998792658</v>
+        <v>0.9973204701</v>
       </c>
       <c r="I66" t="n">
-        <v>14.55386508</v>
+        <v>9.770567506</v>
       </c>
       <c r="J66" t="n">
-        <v>0.243369779</v>
+        <v>0.3400817502</v>
       </c>
       <c r="K66" t="n">
-        <v>0.28447668</v>
+        <v>0.2651975511</v>
       </c>
       <c r="L66" t="n">
-        <v>0.373595397</v>
+        <v>0.3950040297</v>
       </c>
       <c r="M66" t="n">
-        <v>0.017576818</v>
+        <v>0.01755462297</v>
       </c>
     </row>
     <row r="67">
@@ -3308,25 +3308,25 @@
       <c r="E68"/>
       <c r="F68"/>
       <c r="G68" t="n">
-        <v>0.001482654</v>
+        <v>0.001498713878</v>
       </c>
       <c r="H68" t="n">
-        <v>0.998969383</v>
+        <v>0.9984477915</v>
       </c>
       <c r="I68" t="n">
-        <v>24.01503378</v>
+        <v>18.89177552</v>
       </c>
       <c r="J68" t="n">
-        <v>0.36885992</v>
+        <v>0.4243276394</v>
       </c>
       <c r="K68" t="n">
-        <v>0.183429427</v>
+        <v>0.1791966341</v>
       </c>
       <c r="L68" t="n">
-        <v>0.300328179</v>
+        <v>0.3255303847</v>
       </c>
       <c r="M68" t="n">
-        <v>0.018068293</v>
+        <v>0.01807943098</v>
       </c>
     </row>
     <row r="69">
@@ -3380,25 +3380,25 @@
       <c r="E70"/>
       <c r="F70"/>
       <c r="G70" t="n">
-        <v>0.003469694</v>
+        <v>0.003585660708</v>
       </c>
       <c r="H70" t="n">
-        <v>0.998775437</v>
+        <v>0.9973846685</v>
       </c>
       <c r="I70" t="n">
-        <v>20.84387933</v>
+        <v>17.18893711</v>
       </c>
       <c r="J70" t="n">
-        <v>0.391435966</v>
+        <v>0.5294431279</v>
       </c>
       <c r="K70" t="n">
-        <v>0.293413444</v>
+        <v>0.3011933298</v>
       </c>
       <c r="L70" t="n">
-        <v>0.42258362</v>
+        <v>0.4479456515</v>
       </c>
       <c r="M70" t="n">
-        <v>0.018884189</v>
+        <v>0.01893229649</v>
       </c>
     </row>
     <row r="71">
@@ -3452,25 +3452,25 @@
       <c r="E72"/>
       <c r="F72"/>
       <c r="G72" t="n">
-        <v>0.001843514</v>
+        <v>0.001891695447</v>
       </c>
       <c r="H72" t="n">
-        <v>0.998657092</v>
+        <v>0.9988383002</v>
       </c>
       <c r="I72" t="n">
-        <v>12.93881906</v>
+        <v>10.00959712</v>
       </c>
       <c r="J72" t="n">
-        <v>0.467798158</v>
+        <v>0.6605980842</v>
       </c>
       <c r="K72" t="n">
-        <v>0.340552735</v>
+        <v>0.3256696491</v>
       </c>
       <c r="L72" t="n">
-        <v>0.479995679</v>
+        <v>0.4138827043</v>
       </c>
       <c r="M72" t="n">
-        <v>0.017387198</v>
+        <v>0.01738577082</v>
       </c>
     </row>
     <row r="73">
@@ -3524,25 +3524,25 @@
       <c r="E74"/>
       <c r="F74"/>
       <c r="G74" t="n">
-        <v>0.001747159</v>
+        <v>0.001814799783</v>
       </c>
       <c r="H74" t="n">
-        <v>0.998680209</v>
+        <v>0.997794</v>
       </c>
       <c r="I74" t="n">
-        <v>10.92157209</v>
+        <v>8.380991851</v>
       </c>
       <c r="J74" t="n">
-        <v>0.440817926</v>
+        <v>0.5913959046</v>
       </c>
       <c r="K74" t="n">
-        <v>0.525251468</v>
+        <v>0.4931165163</v>
       </c>
       <c r="L74" t="n">
-        <v>0.613802752</v>
+        <v>0.599353621</v>
       </c>
       <c r="M74" t="n">
-        <v>0.018443029</v>
+        <v>0.01847120542</v>
       </c>
     </row>
     <row r="75">
@@ -3596,25 +3596,25 @@
       <c r="E76"/>
       <c r="F76"/>
       <c r="G76" t="n">
-        <v>0.001186751</v>
+        <v>0.0012734324</v>
       </c>
       <c r="H76" t="n">
-        <v>0.998277295</v>
+        <v>0.9983386357</v>
       </c>
       <c r="I76" t="n">
-        <v>11.15392509</v>
+        <v>7.720424386</v>
       </c>
       <c r="J76" t="n">
-        <v>0.308648157</v>
+        <v>0.4739803294</v>
       </c>
       <c r="K76" t="n">
-        <v>0.307433316</v>
+        <v>0.2755574015</v>
       </c>
       <c r="L76" t="n">
-        <v>0.519540666</v>
+        <v>0.486423232</v>
       </c>
       <c r="M76" t="n">
-        <v>0.018014835</v>
+        <v>0.01803366552</v>
       </c>
     </row>
     <row r="77">
@@ -3668,25 +3668,25 @@
       <c r="E78"/>
       <c r="F78"/>
       <c r="G78" t="n">
-        <v>0.002789307</v>
+        <v>0.002914695687</v>
       </c>
       <c r="H78" t="n">
-        <v>0.998732092</v>
+        <v>0.9981671246</v>
       </c>
       <c r="I78" t="n">
-        <v>15.49400055</v>
+        <v>11.28379287</v>
       </c>
       <c r="J78" t="n">
-        <v>0.327538946</v>
+        <v>0.4014873099</v>
       </c>
       <c r="K78" t="n">
-        <v>0.386489339</v>
+        <v>0.4266643684</v>
       </c>
       <c r="L78" t="n">
-        <v>0.511177841</v>
+        <v>0.5620192203</v>
       </c>
       <c r="M78" t="n">
-        <v>0.018289394</v>
+        <v>0.01832784718</v>
       </c>
     </row>
     <row r="79">
@@ -3740,25 +3740,25 @@
       <c r="E80"/>
       <c r="F80"/>
       <c r="G80" t="n">
-        <v>0.005335126</v>
+        <v>0.005525790493</v>
       </c>
       <c r="H80" t="n">
-        <v>0.998549831</v>
+        <v>0.9985826387</v>
       </c>
       <c r="I80" t="n">
-        <v>17.47194325</v>
+        <v>14.28804653</v>
       </c>
       <c r="J80" t="n">
-        <v>0.440817926</v>
+        <v>0.5913959046</v>
       </c>
       <c r="K80" t="n">
-        <v>0.482358105</v>
+        <v>0.496191823</v>
       </c>
       <c r="L80" t="n">
-        <v>0.563775628</v>
+        <v>0.5673957474</v>
       </c>
       <c r="M80" t="n">
-        <v>0.01979391</v>
+        <v>0.01987551916</v>
       </c>
     </row>
     <row r="81">
@@ -3812,25 +3812,25 @@
       <c r="E82"/>
       <c r="F82"/>
       <c r="G82" t="n">
-        <v>0.000882766</v>
+        <v>0.0009543477058</v>
       </c>
       <c r="H82" t="n">
-        <v>0.998192145</v>
+        <v>0.9979762851</v>
       </c>
       <c r="I82" t="n">
-        <v>17.15079447</v>
+        <v>12.91073413</v>
       </c>
       <c r="J82" t="n">
-        <v>0.327538946</v>
+        <v>0.4014873099</v>
       </c>
       <c r="K82" t="n">
-        <v>0.183871997</v>
+        <v>0.1747842113</v>
       </c>
       <c r="L82" t="n">
-        <v>0.403177746</v>
+        <v>0.3650582266</v>
       </c>
       <c r="M82" t="n">
-        <v>0.017907748</v>
+        <v>0.01793683282</v>
       </c>
     </row>
     <row r="83">
@@ -3884,25 +3884,25 @@
       <c r="E84"/>
       <c r="F84"/>
       <c r="G84" t="n">
-        <v>0.001630564</v>
+        <v>0.00161213975</v>
       </c>
       <c r="H84" t="n">
-        <v>0.998554083</v>
+        <v>0.9980941784</v>
       </c>
       <c r="I84" t="n">
-        <v>13.22197373</v>
+        <v>8.844441175</v>
       </c>
       <c r="J84" t="n">
-        <v>0.290846892</v>
+        <v>0.4014873099</v>
       </c>
       <c r="K84" t="n">
-        <v>0.407306292</v>
+        <v>0.4200855213</v>
       </c>
       <c r="L84" t="n">
-        <v>0.485890482</v>
+        <v>0.4741869474</v>
       </c>
       <c r="M84" t="n">
-        <v>0.018078127</v>
+        <v>0.01807787514</v>
       </c>
     </row>
     <row r="85">
@@ -3956,25 +3956,25 @@
       <c r="E86"/>
       <c r="F86"/>
       <c r="G86" t="n">
-        <v>0.001637952</v>
+        <v>0.001734123758</v>
       </c>
       <c r="H86" t="n">
-        <v>0.998199311</v>
+        <v>0.9984521998</v>
       </c>
       <c r="I86" t="n">
-        <v>10.13463639</v>
+        <v>5.934820597</v>
       </c>
       <c r="J86" t="n">
-        <v>0.20364271</v>
+        <v>0.3594287608</v>
       </c>
       <c r="K86" t="n">
-        <v>0.469869735</v>
+        <v>0.2921884299</v>
       </c>
       <c r="L86" t="n">
-        <v>0.596167913</v>
+        <v>0.4422947122</v>
       </c>
       <c r="M86" t="n">
-        <v>0.018215868</v>
+        <v>0.01824423295</v>
       </c>
     </row>
     <row r="87">
@@ -4028,25 +4028,25 @@
       <c r="E88"/>
       <c r="F88"/>
       <c r="G88" t="n">
-        <v>0.001309661</v>
+        <v>0.001399331731</v>
       </c>
       <c r="H88" t="n">
-        <v>0.999138808</v>
+        <v>0.9980484171</v>
       </c>
       <c r="I88" t="n">
-        <v>11.16138579</v>
+        <v>8.336738608</v>
       </c>
       <c r="J88" t="n">
-        <v>0.415393778</v>
+        <v>0.6605980842</v>
       </c>
       <c r="K88" t="n">
-        <v>0.151634155</v>
+        <v>0.1713095657</v>
       </c>
       <c r="L88" t="n">
-        <v>0.303397603</v>
+        <v>0.3319460294</v>
       </c>
       <c r="M88" t="n">
-        <v>0.017616154</v>
+        <v>0.01760490934</v>
       </c>
     </row>
     <row r="89">
@@ -4100,25 +4100,25 @@
       <c r="E90"/>
       <c r="F90"/>
       <c r="G90" t="n">
-        <v>0.00156659</v>
+        <v>0.001586242512</v>
       </c>
       <c r="H90" t="n">
-        <v>0.998632684</v>
+        <v>0.9986190307</v>
       </c>
       <c r="I90" t="n">
-        <v>12.3497021</v>
+        <v>9.248035172</v>
       </c>
       <c r="J90" t="n">
-        <v>0.391435966</v>
+        <v>0.62504</v>
       </c>
       <c r="K90" t="n">
-        <v>0.188480701</v>
+        <v>0.2253715613</v>
       </c>
       <c r="L90" t="n">
-        <v>0.340326428</v>
+        <v>0.3777190835</v>
       </c>
       <c r="M90" t="n">
-        <v>0.017715339</v>
+        <v>0.0177181777</v>
       </c>
     </row>
     <row r="91">
@@ -4172,25 +4172,25 @@
       <c r="E92"/>
       <c r="F92"/>
       <c r="G92" t="n">
-        <v>0.001379314</v>
+        <v>0.001451020175</v>
       </c>
       <c r="H92" t="n">
-        <v>0.999036712</v>
+        <v>0.9977307443</v>
       </c>
       <c r="I92" t="n">
-        <v>14.09405623</v>
+        <v>7.557023733</v>
       </c>
       <c r="J92" t="n">
-        <v>0.160572744</v>
+        <v>0.2308749621</v>
       </c>
       <c r="K92" t="n">
-        <v>0.561422278</v>
+        <v>0.4527713379</v>
       </c>
       <c r="L92" t="n">
-        <v>0.531321491</v>
+        <v>0.4375054281</v>
       </c>
       <c r="M92" t="n">
-        <v>0.017374983</v>
+        <v>0.01733913859</v>
       </c>
     </row>
     <row r="93">
@@ -4244,25 +4244,25 @@
       <c r="E94"/>
       <c r="F94"/>
       <c r="G94" t="n">
-        <v>0.00441708</v>
+        <v>0.004585544796</v>
       </c>
       <c r="H94" t="n">
-        <v>0.998739055</v>
+        <v>0.9986841728</v>
       </c>
       <c r="I94" t="n">
-        <v>10.80511762</v>
+        <v>8.109444765</v>
       </c>
       <c r="J94" t="n">
-        <v>0.347585945</v>
+        <v>0.7378979554</v>
       </c>
       <c r="K94" t="n">
-        <v>0.130091153</v>
+        <v>0.118869778</v>
       </c>
       <c r="L94" t="n">
-        <v>0.355638748</v>
+        <v>0.3686351397</v>
       </c>
       <c r="M94" t="n">
-        <v>0.019459826</v>
+        <v>0.01952852038</v>
       </c>
     </row>
     <row r="95">
@@ -4316,25 +4316,25 @@
       <c r="E96"/>
       <c r="F96"/>
       <c r="G96" t="n">
-        <v>0.005865819</v>
+        <v>0.006056402124</v>
       </c>
       <c r="H96" t="n">
-        <v>0.997985012</v>
+        <v>0.9987079525</v>
       </c>
       <c r="I96" t="n">
-        <v>13.61075036</v>
+        <v>10.39512777</v>
       </c>
       <c r="J96" t="n">
-        <v>0.391435966</v>
+        <v>0.62504</v>
       </c>
       <c r="K96" t="n">
-        <v>0.179356348</v>
+        <v>0.1753398866</v>
       </c>
       <c r="L96" t="n">
-        <v>0.294376554</v>
+        <v>0.3155134442</v>
       </c>
       <c r="M96" t="n">
-        <v>0.020078889</v>
+        <v>0.02016198729</v>
       </c>
     </row>
     <row r="97">
@@ -4388,25 +4388,25 @@
       <c r="E98"/>
       <c r="F98"/>
       <c r="G98" t="n">
-        <v>0.005041598</v>
+        <v>0.005235527417</v>
       </c>
       <c r="H98" t="n">
-        <v>0.998425488</v>
+        <v>0.9982708013</v>
       </c>
       <c r="I98" t="n">
-        <v>11.69816589</v>
+        <v>8.497286328</v>
       </c>
       <c r="J98" t="n">
-        <v>0.308648157</v>
+        <v>0.5913959046</v>
       </c>
       <c r="K98" t="n">
-        <v>0.248884902</v>
+        <v>0.2212102507</v>
       </c>
       <c r="L98" t="n">
-        <v>0.413098254</v>
+        <v>0.391001759</v>
       </c>
       <c r="M98" t="n">
-        <v>0.019722448</v>
+        <v>0.01980409344</v>
       </c>
     </row>
     <row r="99">
@@ -4460,25 +4460,25 @@
       <c r="E100"/>
       <c r="F100"/>
       <c r="G100" t="n">
-        <v>0.00730538</v>
+        <v>0.007515140223</v>
       </c>
       <c r="H100" t="n">
-        <v>0.998486079</v>
+        <v>0.9976183271</v>
       </c>
       <c r="I100" t="n">
-        <v>14.2380775</v>
+        <v>10.85991033</v>
       </c>
       <c r="J100" t="n">
-        <v>0.415393778</v>
+        <v>0.6605980842</v>
       </c>
       <c r="K100" t="n">
-        <v>0.2886548</v>
+        <v>0.2872119023</v>
       </c>
       <c r="L100" t="n">
-        <v>0.337152541</v>
+        <v>0.3813661258</v>
       </c>
       <c r="M100" t="n">
-        <v>0.020693929</v>
+        <v>0.02078594416</v>
       </c>
     </row>
     <row r="101">
@@ -4532,25 +4532,25 @@
       <c r="E102"/>
       <c r="F102"/>
       <c r="G102" t="n">
-        <v>0.005226403</v>
+        <v>0.005417164902</v>
       </c>
       <c r="H102" t="n">
-        <v>0.999065791</v>
+        <v>0.9981681785</v>
       </c>
       <c r="I102" t="n">
-        <v>21.29207659</v>
+        <v>16.67553361</v>
       </c>
       <c r="J102" t="n">
-        <v>0.415393778</v>
+        <v>0.5294431279</v>
       </c>
       <c r="K102" t="n">
-        <v>0.24476547</v>
+        <v>0.2518589921</v>
       </c>
       <c r="L102" t="n">
-        <v>0.38799953</v>
+        <v>0.4136666028</v>
       </c>
       <c r="M102" t="n">
-        <v>0.019840586</v>
+        <v>0.01993099998</v>
       </c>
     </row>
     <row r="103">
@@ -4604,25 +4604,25 @@
       <c r="E104"/>
       <c r="F104"/>
       <c r="G104" t="n">
-        <v>0.005607542</v>
+        <v>0.005813407676</v>
       </c>
       <c r="H104" t="n">
-        <v>0.999001959</v>
+        <v>0.9977098276</v>
       </c>
       <c r="I104" t="n">
-        <v>20.37145918</v>
+        <v>16.51537209</v>
       </c>
       <c r="J104" t="n">
-        <v>0.36885992</v>
+        <v>0.62504</v>
       </c>
       <c r="K104" t="n">
-        <v>0.206435076</v>
+        <v>0.196151054</v>
       </c>
       <c r="L104" t="n">
-        <v>0.409168761</v>
+        <v>0.415156062</v>
       </c>
       <c r="M104" t="n">
-        <v>0.020035127</v>
+        <v>0.02012573649</v>
       </c>
     </row>
     <row r="105">
@@ -4676,25 +4676,25 @@
       <c r="E106"/>
       <c r="F106"/>
       <c r="G106" t="n">
-        <v>0.006435156</v>
+        <v>0.006676155159</v>
       </c>
       <c r="H106" t="n">
-        <v>0.99823614</v>
+        <v>0.9988392089</v>
       </c>
       <c r="I106" t="n">
-        <v>12.76960462</v>
+        <v>9.261988616</v>
       </c>
       <c r="J106" t="n">
-        <v>0.327538946</v>
+        <v>0.5913959046</v>
       </c>
       <c r="K106" t="n">
-        <v>0.211535812</v>
+        <v>0.2436289336</v>
       </c>
       <c r="L106" t="n">
-        <v>0.38758931</v>
+        <v>0.4312631198</v>
       </c>
       <c r="M106" t="n">
-        <v>0.020441863</v>
+        <v>0.02054430432</v>
       </c>
     </row>
     <row r="107">
@@ -4748,25 +4748,25 @@
       <c r="E108"/>
       <c r="F108"/>
       <c r="G108" t="n">
-        <v>0.005030818</v>
+        <v>0.005205715898</v>
       </c>
       <c r="H108" t="n">
-        <v>0.9977707</v>
+        <v>0.9984887844</v>
       </c>
       <c r="I108" t="n">
-        <v>10.55356265</v>
+        <v>6.752552626</v>
       </c>
       <c r="J108" t="n">
-        <v>0.229333441</v>
+        <v>0.4014873099</v>
       </c>
       <c r="K108" t="n">
-        <v>0.20098465</v>
+        <v>0.1858837352</v>
       </c>
       <c r="L108" t="n">
-        <v>0.314306336</v>
+        <v>0.3129862979</v>
       </c>
       <c r="M108" t="n">
-        <v>0.019758475</v>
+        <v>0.01983216209</v>
       </c>
     </row>
     <row r="109">
@@ -4820,25 +4820,25 @@
       <c r="E110"/>
       <c r="F110"/>
       <c r="G110" t="n">
-        <v>0.006165259</v>
+        <v>0.006389464125</v>
       </c>
       <c r="H110" t="n">
-        <v>0.997936765</v>
+        <v>0.9981549634</v>
       </c>
       <c r="I110" t="n">
-        <v>12.16203353</v>
+        <v>8.635753477</v>
       </c>
       <c r="J110" t="n">
-        <v>0.308648157</v>
+        <v>0.5913959046</v>
       </c>
       <c r="K110" t="n">
-        <v>0.170040492</v>
+        <v>0.1578384252</v>
       </c>
       <c r="L110" t="n">
-        <v>0.387622024</v>
+        <v>0.363770321</v>
       </c>
       <c r="M110" t="n">
-        <v>0.020159258</v>
+        <v>0.0202581831</v>
       </c>
     </row>
     <row r="111">
@@ -4892,25 +4892,25 @@
       <c r="E112"/>
       <c r="F112"/>
       <c r="G112" t="n">
-        <v>0.005658562</v>
+        <v>0.005852936256</v>
       </c>
       <c r="H112" t="n">
-        <v>0.998474708</v>
+        <v>0.9977921317</v>
       </c>
       <c r="I112" t="n">
-        <v>18.69494231</v>
+        <v>14.00007019</v>
       </c>
       <c r="J112" t="n">
-        <v>0.36885992</v>
+        <v>0.4484673392</v>
       </c>
       <c r="K112" t="n">
-        <v>0.174550024</v>
+        <v>0.1926074796</v>
       </c>
       <c r="L112" t="n">
-        <v>0.335602576</v>
+        <v>0.3605887212</v>
       </c>
       <c r="M112" t="n">
-        <v>0.020035173</v>
+        <v>0.02011730976</v>
       </c>
     </row>
     <row r="113">
@@ -4964,25 +4964,25 @@
       <c r="E114"/>
       <c r="F114"/>
       <c r="G114" t="n">
-        <v>0.005218858</v>
+        <v>0.005427667653</v>
       </c>
       <c r="H114" t="n">
-        <v>0.998982101</v>
+        <v>0.9982465489</v>
       </c>
       <c r="I114" t="n">
-        <v>15.30830802</v>
+        <v>11.43827058</v>
       </c>
       <c r="J114" t="n">
-        <v>0.391435966</v>
+        <v>0.5595627735</v>
       </c>
       <c r="K114" t="n">
-        <v>0.222503547</v>
+        <v>0.2262723102</v>
       </c>
       <c r="L114" t="n">
-        <v>0.310358895</v>
+        <v>0.2909851406</v>
       </c>
       <c r="M114" t="n">
-        <v>0.019782696</v>
+        <v>0.01987080113</v>
       </c>
     </row>
     <row r="115">
@@ -5036,25 +5036,25 @@
       <c r="E116"/>
       <c r="F116"/>
       <c r="G116" t="n">
-        <v>0.006188047</v>
+        <v>0.006473264986</v>
       </c>
       <c r="H116" t="n">
-        <v>0.998584048</v>
+        <v>0.9983875073</v>
       </c>
       <c r="I116" t="n">
-        <v>17.64693879</v>
+        <v>12.68285896</v>
       </c>
       <c r="J116" t="n">
-        <v>0.308648157</v>
+        <v>0.4484673392</v>
       </c>
       <c r="K116" t="n">
-        <v>0.276502873</v>
+        <v>0.3095299721</v>
       </c>
       <c r="L116" t="n">
-        <v>0.374478213</v>
+        <v>0.4230375989</v>
       </c>
       <c r="M116" t="n">
-        <v>0.020297027</v>
+        <v>0.02041790809</v>
       </c>
     </row>
     <row r="117">
@@ -5108,25 +5108,25 @@
       <c r="E118"/>
       <c r="F118"/>
       <c r="G118" t="n">
-        <v>0.002936327</v>
+        <v>0.003078460776</v>
       </c>
       <c r="H118" t="n">
-        <v>0.999553351</v>
+        <v>0.9985109531</v>
       </c>
       <c r="I118" t="n">
-        <v>25.27910623</v>
+        <v>21.53721832</v>
       </c>
       <c r="J118" t="n">
-        <v>0.440817926</v>
+        <v>0.62504</v>
       </c>
       <c r="K118" t="n">
-        <v>0.137596898</v>
+        <v>0.1940337857</v>
       </c>
       <c r="L118" t="n">
-        <v>0.348979132</v>
+        <v>0.4208601479</v>
       </c>
       <c r="M118" t="n">
-        <v>0.018769595</v>
+        <v>0.01882726172</v>
       </c>
     </row>
     <row r="119">
@@ -5180,25 +5180,25 @@
       <c r="E120"/>
       <c r="F120"/>
       <c r="G120" t="n">
-        <v>0.005330964</v>
+        <v>0.005571783206</v>
       </c>
       <c r="H120" t="n">
-        <v>0.998908944</v>
+        <v>0.9983165639</v>
       </c>
       <c r="I120" t="n">
-        <v>26.81552944</v>
+        <v>22.49442445</v>
       </c>
       <c r="J120" t="n">
-        <v>0.415393778</v>
+        <v>0.5913959046</v>
       </c>
       <c r="K120" t="n">
-        <v>0.226632057</v>
+        <v>0.20357463</v>
       </c>
       <c r="L120" t="n">
-        <v>0.387700459</v>
+        <v>0.4446905242</v>
       </c>
       <c r="M120" t="n">
-        <v>0.0198376</v>
+        <v>0.0199410144</v>
       </c>
     </row>
     <row r="121">
@@ -5252,25 +5252,25 @@
       <c r="E122"/>
       <c r="F122"/>
       <c r="G122" t="n">
-        <v>0.003954074</v>
+        <v>0.004157924971</v>
       </c>
       <c r="H122" t="n">
-        <v>0.999350198</v>
+        <v>0.9978559964</v>
       </c>
       <c r="I122" t="n">
-        <v>26.42835785</v>
+        <v>21.5657584</v>
       </c>
       <c r="J122" t="n">
-        <v>0.327538946</v>
+        <v>0.4484673392</v>
       </c>
       <c r="K122" t="n">
-        <v>0.244915358</v>
+        <v>0.2684457761</v>
       </c>
       <c r="L122" t="n">
-        <v>0.363960202</v>
+        <v>0.3963223034</v>
       </c>
       <c r="M122" t="n">
-        <v>0.019189749</v>
+        <v>0.01926688936</v>
       </c>
     </row>
     <row r="123">
@@ -5324,25 +5324,25 @@
       <c r="E124"/>
       <c r="F124"/>
       <c r="G124" t="n">
-        <v>0.005712061</v>
+        <v>0.005964065135</v>
       </c>
       <c r="H124" t="n">
-        <v>0.998586302</v>
+        <v>0.9983381879</v>
       </c>
       <c r="I124" t="n">
-        <v>17.38413457</v>
+        <v>12.49190368</v>
       </c>
       <c r="J124" t="n">
-        <v>0.308648157</v>
+        <v>0.4243276394</v>
       </c>
       <c r="K124" t="n">
-        <v>0.237942264</v>
+        <v>0.2784769372</v>
       </c>
       <c r="L124" t="n">
-        <v>0.450188396</v>
+        <v>0.4859585013</v>
       </c>
       <c r="M124" t="n">
-        <v>0.019987</v>
+        <v>0.02009966669</v>
       </c>
     </row>
     <row r="125">
@@ -5396,25 +5396,25 @@
       <c r="E126"/>
       <c r="F126"/>
       <c r="G126" t="n">
-        <v>0.004297867</v>
+        <v>0.004502523068</v>
       </c>
       <c r="H126" t="n">
-        <v>0.998051701</v>
+        <v>0.9984773986</v>
       </c>
       <c r="I126" t="n">
-        <v>10.53507997</v>
+        <v>7.270033034</v>
       </c>
       <c r="J126" t="n">
-        <v>0.308648157</v>
+        <v>0.4243276394</v>
       </c>
       <c r="K126" t="n">
-        <v>0.182136417</v>
+        <v>0.2022066066</v>
       </c>
       <c r="L126" t="n">
-        <v>0.281043188</v>
+        <v>0.3005931159</v>
       </c>
       <c r="M126" t="n">
-        <v>0.019470585</v>
+        <v>0.01955734737</v>
       </c>
     </row>
     <row r="127">
@@ -5468,25 +5468,25 @@
       <c r="E128"/>
       <c r="F128"/>
       <c r="G128" t="n">
-        <v>0.005007014</v>
+        <v>0.005205144759</v>
       </c>
       <c r="H128" t="n">
-        <v>0.997851199</v>
+        <v>0.9985081059</v>
       </c>
       <c r="I128" t="n">
-        <v>12.18297185</v>
+        <v>8.653693862</v>
       </c>
       <c r="J128" t="n">
-        <v>0.308648157</v>
+        <v>0.62504</v>
       </c>
       <c r="K128" t="n">
-        <v>0.153521693</v>
+        <v>0.1488538869</v>
       </c>
       <c r="L128" t="n">
-        <v>0.321201434</v>
+        <v>0.3698596561</v>
       </c>
       <c r="M128" t="n">
-        <v>0.019777487</v>
+        <v>0.01986150023</v>
       </c>
     </row>
     <row r="129">
@@ -5540,25 +5540,25 @@
       <c r="E130"/>
       <c r="F130"/>
       <c r="G130" t="n">
-        <v>0.00477814</v>
+        <v>0.004997248187</v>
       </c>
       <c r="H130" t="n">
-        <v>0.997718162</v>
+        <v>0.998354787</v>
       </c>
       <c r="I130" t="n">
-        <v>12.12069114</v>
+        <v>8.089687639</v>
       </c>
       <c r="J130" t="n">
-        <v>0.308648157</v>
+        <v>0.4014873099</v>
       </c>
       <c r="K130" t="n">
-        <v>0.155917005</v>
+        <v>0.1630998168</v>
       </c>
       <c r="L130" t="n">
-        <v>0.251486818</v>
+        <v>0.2920514371</v>
       </c>
       <c r="M130" t="n">
-        <v>0.019684972</v>
+        <v>0.01977622094</v>
       </c>
     </row>
     <row r="131">
@@ -5612,25 +5612,25 @@
       <c r="E132"/>
       <c r="F132"/>
       <c r="G132" t="n">
-        <v>0.006244524</v>
+        <v>0.006495825812</v>
       </c>
       <c r="H132" t="n">
-        <v>0.998104698</v>
+        <v>0.9983295065</v>
       </c>
       <c r="I132" t="n">
-        <v>12.20842257</v>
+        <v>8.663931859</v>
       </c>
       <c r="J132" t="n">
-        <v>0.327538946</v>
+        <v>0.5294431279</v>
       </c>
       <c r="K132" t="n">
-        <v>0.124791542</v>
+        <v>0.1596243399</v>
       </c>
       <c r="L132" t="n">
-        <v>0.422103071</v>
+        <v>0.4685799982</v>
       </c>
       <c r="M132" t="n">
-        <v>0.020199117</v>
+        <v>0.02030420169</v>
       </c>
     </row>
     <row r="133">
@@ -5684,25 +5684,25 @@
       <c r="E134"/>
       <c r="F134"/>
       <c r="G134" t="n">
-        <v>0.003686526</v>
+        <v>0.003842879113</v>
       </c>
       <c r="H134" t="n">
-        <v>0.998850503</v>
+        <v>0.9982269937</v>
       </c>
       <c r="I134" t="n">
-        <v>32.31299832</v>
+        <v>28.0022206</v>
       </c>
       <c r="J134" t="n">
-        <v>0.52681366</v>
+        <v>0.5913959046</v>
       </c>
       <c r="K134" t="n">
-        <v>0.221627398</v>
+        <v>0.2439080387</v>
       </c>
       <c r="L134" t="n">
-        <v>0.376795751</v>
+        <v>0.4055769628</v>
       </c>
       <c r="M134" t="n">
-        <v>0.019115734</v>
+        <v>0.01918915417</v>
       </c>
     </row>
     <row r="135">
@@ -5756,25 +5756,25 @@
       <c r="E136"/>
       <c r="F136"/>
       <c r="G136" t="n">
-        <v>0.005382125</v>
+        <v>0.005630646001</v>
       </c>
       <c r="H136" t="n">
-        <v>0.998834003</v>
+        <v>0.9977694499</v>
       </c>
       <c r="I136" t="n">
-        <v>19.87383246</v>
+        <v>15.24439242</v>
       </c>
       <c r="J136" t="n">
-        <v>0.36885992</v>
+        <v>0.4484673392</v>
       </c>
       <c r="K136" t="n">
-        <v>0.262633309</v>
+        <v>0.2632266342</v>
       </c>
       <c r="L136" t="n">
-        <v>0.414915744</v>
+        <v>0.418701688</v>
       </c>
       <c r="M136" t="n">
-        <v>0.019843407</v>
+        <v>0.01995069442</v>
       </c>
     </row>
     <row r="137">
@@ -5828,25 +5828,25 @@
       <c r="E138"/>
       <c r="F138"/>
       <c r="G138" t="n">
-        <v>0.003443489</v>
+        <v>0.003611205844</v>
       </c>
       <c r="H138" t="n">
-        <v>0.99858164</v>
+        <v>0.9978901187</v>
       </c>
       <c r="I138" t="n">
-        <v>21.76531836</v>
+        <v>17.03755774</v>
       </c>
       <c r="J138" t="n">
-        <v>0.36885992</v>
+        <v>0.4243276394</v>
       </c>
       <c r="K138" t="n">
-        <v>0.208026749</v>
+        <v>0.2435244304</v>
       </c>
       <c r="L138" t="n">
-        <v>0.38001658</v>
+        <v>0.383738795</v>
       </c>
       <c r="M138" t="n">
-        <v>0.019077701</v>
+        <v>0.01915084821</v>
       </c>
     </row>
     <row r="139">
@@ -5900,25 +5900,25 @@
       <c r="E140"/>
       <c r="F140"/>
       <c r="G140" t="n">
-        <v>0.003670018</v>
+        <v>0.003841199745</v>
       </c>
       <c r="H140" t="n">
-        <v>0.999164383</v>
+        <v>0.9986899036</v>
       </c>
       <c r="I140" t="n">
-        <v>22.00180447</v>
+        <v>17.57807132</v>
       </c>
       <c r="J140" t="n">
-        <v>0.36885992</v>
+        <v>0.5913959046</v>
       </c>
       <c r="K140" t="n">
-        <v>0.284540459</v>
+        <v>0.2801415148</v>
       </c>
       <c r="L140" t="n">
-        <v>0.325526873</v>
+        <v>0.3365741565</v>
       </c>
       <c r="M140" t="n">
-        <v>0.019060035</v>
+        <v>0.01913220536</v>
       </c>
     </row>
     <row r="141">
@@ -5974,25 +5974,25 @@
         <v>92</v>
       </c>
       <c r="G142" t="n">
-        <v>0.001086565</v>
+        <v>0.00112382419</v>
       </c>
       <c r="H142" t="n">
-        <v>0.998310517</v>
+        <v>0.9649402231</v>
       </c>
       <c r="I142" t="n">
-        <v>42.47753596</v>
+        <v>33.25588838</v>
       </c>
       <c r="J142" t="n">
-        <v>0.098273676</v>
+        <v>0.1487768382</v>
       </c>
       <c r="K142" t="n">
-        <v>0.115494724</v>
+        <v>0.1320614168</v>
       </c>
       <c r="L142" t="n">
-        <v>0.181728511</v>
+        <v>0.2277337819</v>
       </c>
       <c r="M142" t="n">
-        <v>0.017208908</v>
+        <v>0.01719386889</v>
       </c>
     </row>
     <row r="143">
@@ -6050,25 +6050,25 @@
         <v>92</v>
       </c>
       <c r="G144" t="n">
-        <v>0.001686946</v>
+        <v>0.001747799759</v>
       </c>
       <c r="H144" t="n">
-        <v>0.998181677</v>
+        <v>0.9645403369</v>
       </c>
       <c r="I144" t="n">
-        <v>38.86831145</v>
+        <v>30.30262563</v>
       </c>
       <c r="J144" t="n">
-        <v>0.098273676</v>
+        <v>0.1487768382</v>
       </c>
       <c r="K144" t="n">
-        <v>0.144772861</v>
+        <v>0.1480684212</v>
       </c>
       <c r="L144" t="n">
-        <v>0.191527528</v>
+        <v>0.2414522146</v>
       </c>
       <c r="M144" t="n">
-        <v>0.017373607</v>
+        <v>0.01737157543</v>
       </c>
     </row>
     <row r="145">
@@ -6126,25 +6126,25 @@
         <v>95</v>
       </c>
       <c r="G146" t="n">
-        <v>0.001438974</v>
+        <v>0.001501163817</v>
       </c>
       <c r="H146" t="n">
-        <v>0.998274232</v>
+        <v>0.9640799439</v>
       </c>
       <c r="I146" t="n">
-        <v>45.35369521</v>
+        <v>35.35793006</v>
       </c>
       <c r="J146" t="n">
-        <v>0.098273676</v>
+        <v>0.1487768382</v>
       </c>
       <c r="K146" t="n">
-        <v>0.1065651</v>
+        <v>0.1188221864</v>
       </c>
       <c r="L146" t="n">
-        <v>0.159267507</v>
+        <v>0.2011162269</v>
       </c>
       <c r="M146" t="n">
-        <v>0.017082766</v>
+        <v>0.01706059375</v>
       </c>
     </row>
     <row r="147">
@@ -6202,25 +6202,25 @@
         <v>95</v>
       </c>
       <c r="G148" t="n">
-        <v>0.0000187</v>
+        <v>0.00003663171778</v>
       </c>
       <c r="H148" t="n">
-        <v>0.998017587</v>
+        <v>0.9622675292</v>
       </c>
       <c r="I148" t="n">
-        <v>41.7451596</v>
+        <v>32.21166602</v>
       </c>
       <c r="J148" t="n">
-        <v>0.090676075</v>
+        <v>0.1487768382</v>
       </c>
       <c r="K148" t="n">
-        <v>0.098946404</v>
+        <v>0.112306445</v>
       </c>
       <c r="L148" t="n">
-        <v>0.15843918</v>
+        <v>0.2023010249</v>
       </c>
       <c r="M148" t="n">
-        <v>0.017661164</v>
+        <v>0.01765956395</v>
       </c>
     </row>
     <row r="149">
@@ -6278,25 +6278,25 @@
         <v>92</v>
       </c>
       <c r="G150" t="n">
-        <v>0.001032382</v>
+        <v>0.001047685475</v>
       </c>
       <c r="H150" t="n">
-        <v>0.998208141</v>
+        <v>0.9541553811</v>
       </c>
       <c r="I150" t="n">
-        <v>45.64855025</v>
+        <v>35.77846642</v>
       </c>
       <c r="J150" t="n">
-        <v>0.098273676</v>
+        <v>0.1487768382</v>
       </c>
       <c r="K150" t="n">
-        <v>0.091605465</v>
+        <v>0.1001065453</v>
       </c>
       <c r="L150" t="n">
-        <v>0.12475774</v>
+        <v>0.1573114157</v>
       </c>
       <c r="M150" t="n">
-        <v>0.017488338</v>
+        <v>0.01748989717</v>
       </c>
     </row>
     <row r="151">
@@ -6354,25 +6354,25 @@
         <v>92</v>
       </c>
       <c r="G152" t="n">
-        <v>0.001059082</v>
+        <v>0.00109272312</v>
       </c>
       <c r="H152" t="n">
-        <v>0.998117027</v>
+        <v>0.954819135</v>
       </c>
       <c r="I152" t="n">
-        <v>42.47218426</v>
+        <v>32.634796</v>
       </c>
       <c r="J152" t="n">
-        <v>0.090676075</v>
+        <v>0.1487768382</v>
       </c>
       <c r="K152" t="n">
-        <v>0.108206556</v>
+        <v>0.1133424315</v>
       </c>
       <c r="L152" t="n">
-        <v>0.156468717</v>
+        <v>0.1922152256</v>
       </c>
       <c r="M152" t="n">
-        <v>0.017380662</v>
+        <v>0.01737567955</v>
       </c>
     </row>
     <row r="153">
@@ -6430,25 +6430,25 @@
         <v>95</v>
       </c>
       <c r="G154" t="n">
-        <v>0.001075488</v>
+        <v>0.001090874277</v>
       </c>
       <c r="H154" t="n">
-        <v>0.998463534</v>
+        <v>0.9994579584</v>
       </c>
       <c r="I154" t="n">
-        <v>20.28081709</v>
+        <v>20.50910277</v>
       </c>
       <c r="J154" t="n">
-        <v>0.172603108</v>
+        <v>2.926507403</v>
       </c>
       <c r="K154" t="n">
-        <v>0.142220048</v>
+        <v>0.1721985212</v>
       </c>
       <c r="L154" t="n">
-        <v>0.216962845</v>
+        <v>0.2612446632</v>
       </c>
       <c r="M154" t="n">
-        <v>0.017516242</v>
+        <v>0.01751697706</v>
       </c>
     </row>
     <row r="155">
@@ -6506,25 +6506,25 @@
         <v>95</v>
       </c>
       <c r="G156" t="n">
-        <v>0.003466463</v>
+        <v>0.003526645148</v>
       </c>
       <c r="H156" t="n">
-        <v>0.99807401</v>
+        <v>0.9781051126</v>
       </c>
       <c r="I156" t="n">
-        <v>43.67214478</v>
+        <v>36.05329534</v>
       </c>
       <c r="J156" t="n">
-        <v>0.125103846</v>
+        <v>0.1487768382</v>
       </c>
       <c r="K156" t="n">
-        <v>0.090791297</v>
+        <v>0.1166349597</v>
       </c>
       <c r="L156" t="n">
-        <v>0.221010255</v>
+        <v>0.2697936088</v>
       </c>
       <c r="M156" t="n">
-        <v>0.01786269</v>
+        <v>0.01789620905</v>
       </c>
     </row>
     <row r="157">
@@ -6582,25 +6582,25 @@
         <v>92</v>
       </c>
       <c r="G158" t="n">
-        <v>0.000767719</v>
+        <v>0.0007873147174</v>
       </c>
       <c r="H158" t="n">
-        <v>0.998024578</v>
+        <v>0.9687007925</v>
       </c>
       <c r="I158" t="n">
-        <v>42.18953537</v>
+        <v>32.93456721</v>
       </c>
       <c r="J158" t="n">
-        <v>0.098273676</v>
+        <v>0.1487768382</v>
       </c>
       <c r="K158" t="n">
-        <v>0.154945531</v>
+        <v>0.1648586724</v>
       </c>
       <c r="L158" t="n">
-        <v>0.196330737</v>
+        <v>0.2494563427</v>
       </c>
       <c r="M158" t="n">
-        <v>0.017367301</v>
+        <v>0.01735927631</v>
       </c>
     </row>
     <row r="159">
@@ -6658,25 +6658,25 @@
         <v>95</v>
       </c>
       <c r="G160" t="n">
-        <v>0.000828315</v>
+        <v>0.0008689380972</v>
       </c>
       <c r="H160" t="n">
-        <v>0.998384972</v>
+        <v>0.9668825284</v>
       </c>
       <c r="I160" t="n">
-        <v>46.23666979</v>
+        <v>36.60732582</v>
       </c>
       <c r="J160" t="n">
-        <v>0.098273676</v>
+        <v>0.1487768382</v>
       </c>
       <c r="K160" t="n">
-        <v>0.176976089</v>
+        <v>0.1969198415</v>
       </c>
       <c r="L160" t="n">
-        <v>0.214938239</v>
+        <v>0.2576204095</v>
       </c>
       <c r="M160" t="n">
-        <v>0.017335313</v>
+        <v>0.0173196805</v>
       </c>
     </row>
     <row r="161">
@@ -6734,25 +6734,25 @@
         <v>92</v>
       </c>
       <c r="G162" t="n">
-        <v>0.001235508</v>
+        <v>0.001351616979</v>
       </c>
       <c r="H162" t="n">
-        <v>0.998403963</v>
+        <v>0.9969253405</v>
       </c>
       <c r="I162" t="n">
-        <v>37.83424722</v>
+        <v>33.3489681</v>
       </c>
       <c r="J162" t="n">
-        <v>0.146946632</v>
+        <v>0.1487768382</v>
       </c>
       <c r="K162" t="n">
-        <v>0.120464395</v>
+        <v>0.1078059316</v>
       </c>
       <c r="L162" t="n">
-        <v>0.130787072</v>
+        <v>0.1681378255</v>
       </c>
       <c r="M162" t="n">
-        <v>0.017451291</v>
+        <v>0.01746284442</v>
       </c>
     </row>
     <row r="163">
@@ -6810,25 +6810,25 @@
         <v>92</v>
       </c>
       <c r="G164" t="n">
-        <v>0.000824688</v>
+        <v>0.0007937613179</v>
       </c>
       <c r="H164" t="n">
-        <v>0.998297541</v>
+        <v>0.9942276257</v>
       </c>
       <c r="I164" t="n">
-        <v>42.8669483</v>
+        <v>35.67569033</v>
       </c>
       <c r="J164" t="n">
-        <v>0.125103846</v>
+        <v>0.1487768382</v>
       </c>
       <c r="K164" t="n">
-        <v>0.128896908</v>
+        <v>0.1370265821</v>
       </c>
       <c r="L164" t="n">
-        <v>0.167566418</v>
+        <v>0.2350099549</v>
       </c>
       <c r="M164" t="n">
-        <v>0.017481459</v>
+        <v>0.01748640034</v>
       </c>
     </row>
     <row r="165">
@@ -6886,25 +6886,25 @@
         <v>95</v>
       </c>
       <c r="G166" t="n">
-        <v>0.001438861</v>
+        <v>0.001386859646</v>
       </c>
       <c r="H166" t="n">
-        <v>0.998011514</v>
+        <v>0.9759773096</v>
       </c>
       <c r="I166" t="n">
-        <v>44.52845104</v>
+        <v>36.118567</v>
       </c>
       <c r="J166" t="n">
-        <v>0.115431988</v>
+        <v>0.1487768382</v>
       </c>
       <c r="K166" t="n">
-        <v>0.128309112</v>
+        <v>0.1486066244</v>
       </c>
       <c r="L166" t="n">
-        <v>0.184525757</v>
+        <v>0.2249090762</v>
       </c>
       <c r="M166" t="n">
-        <v>0.01764173</v>
+        <v>0.01762566378</v>
       </c>
     </row>
     <row r="167">
@@ -6962,25 +6962,25 @@
         <v>95</v>
       </c>
       <c r="G168" t="n">
-        <v>0.000479482</v>
+        <v>0.000491684713</v>
       </c>
       <c r="H168" t="n">
-        <v>0.99812104</v>
+        <v>0.9744148084</v>
       </c>
       <c r="I168" t="n">
-        <v>46.6709541</v>
+        <v>37.2777845</v>
       </c>
       <c r="J168" t="n">
-        <v>0.106507867</v>
+        <v>0.1487768382</v>
       </c>
       <c r="K168" t="n">
-        <v>0.092286484</v>
+        <v>0.100009045</v>
       </c>
       <c r="L168" t="n">
-        <v>0.132139707</v>
+        <v>0.1524915323</v>
       </c>
       <c r="M168" t="n">
-        <v>0.017740057</v>
+        <v>0.01774240393</v>
       </c>
     </row>
     <row r="169">
@@ -7038,25 +7038,25 @@
         <v>92</v>
       </c>
       <c r="G170" t="n">
-        <v>0.00282281</v>
+        <v>0.002593926772</v>
       </c>
       <c r="H170" t="n">
-        <v>0.999493818</v>
+        <v>0.9981351597</v>
       </c>
       <c r="I170" t="n">
-        <v>28.19223751</v>
+        <v>28.70130293</v>
       </c>
       <c r="J170" t="n">
-        <v>29.75060383</v>
+        <v>28.9461893</v>
       </c>
       <c r="K170" t="n">
-        <v>0.299872426</v>
+        <v>0.4137206222</v>
       </c>
       <c r="L170" t="n">
-        <v>0.52126036</v>
+        <v>0.8136697615</v>
       </c>
       <c r="M170" t="n">
-        <v>0.018389595</v>
+        <v>0.01845064221</v>
       </c>
     </row>
     <row r="171">
@@ -7114,25 +7114,25 @@
         <v>92</v>
       </c>
       <c r="G172" t="n">
-        <v>0.002873698</v>
+        <v>0.003139539945</v>
       </c>
       <c r="H172" t="n">
-        <v>0.998937611</v>
+        <v>0.9981270834</v>
       </c>
       <c r="I172" t="n">
-        <v>27.83710297</v>
+        <v>27.60120501</v>
       </c>
       <c r="J172" t="n">
-        <v>0.098273676</v>
+        <v>19.75685304</v>
       </c>
       <c r="K172" t="n">
-        <v>0.255040755</v>
+        <v>0.4189861196</v>
       </c>
       <c r="L172" t="n">
-        <v>0.408088731</v>
+        <v>0.6517685002</v>
       </c>
       <c r="M172" t="n">
-        <v>0.018695971</v>
+        <v>0.01881955794</v>
       </c>
     </row>
     <row r="173">
@@ -7190,25 +7190,25 @@
         <v>95</v>
       </c>
       <c r="G174" t="n">
-        <v>0.001005804</v>
+        <v>0.001104559584</v>
       </c>
       <c r="H174" t="n">
-        <v>0.998849444</v>
+        <v>0.9983590376</v>
       </c>
       <c r="I174" t="n">
-        <v>43.16705597</v>
+        <v>44.00594144</v>
       </c>
       <c r="J174" t="n">
-        <v>6.990287164</v>
+        <v>15.7106297</v>
       </c>
       <c r="K174" t="n">
-        <v>0.38441635</v>
+        <v>0.3765886809</v>
       </c>
       <c r="L174" t="n">
-        <v>0.679881647</v>
+        <v>0.7504292451</v>
       </c>
       <c r="M174" t="n">
-        <v>0.018006318</v>
+        <v>0.01807606708</v>
       </c>
     </row>
     <row r="175">
@@ -7266,25 +7266,25 @@
         <v>95</v>
       </c>
       <c r="G176" t="n">
-        <v>0.004908073</v>
+        <v>0.00520758282</v>
       </c>
       <c r="H176" t="n">
-        <v>0.998885923</v>
+        <v>0.9977955808</v>
       </c>
       <c r="I176" t="n">
-        <v>52.15774541</v>
+        <v>51.36728127</v>
       </c>
       <c r="J176" t="n">
-        <v>0.453296594</v>
+        <v>0.2352792781</v>
       </c>
       <c r="K176" t="n">
-        <v>0.477906688</v>
+        <v>0.414137293</v>
       </c>
       <c r="L176" t="n">
-        <v>0.693555248</v>
+        <v>0.6662992199</v>
       </c>
       <c r="M176" t="n">
-        <v>0.019741438</v>
+        <v>0.01989473552</v>
       </c>
     </row>
     <row r="177">
@@ -7342,25 +7342,25 @@
         <v>92</v>
       </c>
       <c r="G178" t="n">
-        <v>0.000343256</v>
+        <v>0.0002936432628</v>
       </c>
       <c r="H178" t="n">
-        <v>0.998742978</v>
+        <v>0.9970862742</v>
       </c>
       <c r="I178" t="n">
-        <v>44.77321715</v>
+        <v>40.92243128</v>
       </c>
       <c r="J178" t="n">
-        <v>0.279714856</v>
+        <v>0.2352792781</v>
       </c>
       <c r="K178" t="n">
-        <v>0.310355073</v>
+        <v>0.2825431635</v>
       </c>
       <c r="L178" t="n">
-        <v>0.416775242</v>
+        <v>0.3971300607</v>
       </c>
       <c r="M178" t="n">
-        <v>0.017659969</v>
+        <v>0.01763152028</v>
       </c>
     </row>
     <row r="179">
@@ -7418,25 +7418,25 @@
         <v>92</v>
       </c>
       <c r="G180" t="n">
-        <v>0.000868187</v>
+        <v>0.000919971656</v>
       </c>
       <c r="H180" t="n">
-        <v>0.99800771</v>
+        <v>0.9975038456</v>
       </c>
       <c r="I180" t="n">
-        <v>52.56948935</v>
+        <v>48.65456508</v>
       </c>
       <c r="J180" t="n">
-        <v>0.418251945</v>
+        <v>0.3720763218</v>
       </c>
       <c r="K180" t="n">
-        <v>0.262397919</v>
+        <v>0.2722140138</v>
       </c>
       <c r="L180" t="n">
-        <v>0.445268964</v>
+        <v>0.4869355776</v>
       </c>
       <c r="M180" t="n">
-        <v>0.018009401</v>
+        <v>0.01802049863</v>
       </c>
     </row>
     <row r="181">
@@ -7494,25 +7494,25 @@
         <v>95</v>
       </c>
       <c r="G182" t="n">
-        <v>0.001727267</v>
+        <v>0.002119448847</v>
       </c>
       <c r="H182" t="n">
-        <v>0.983654412</v>
+        <v>0.9753035996</v>
       </c>
       <c r="I182" t="n">
-        <v>53.74611704</v>
+        <v>57.90574331</v>
       </c>
       <c r="J182" t="n">
-        <v>241.0196487</v>
+        <v>106.0624695</v>
       </c>
       <c r="K182" t="n">
-        <v>1.292871138</v>
+        <v>0.9607836648</v>
       </c>
       <c r="L182" t="n">
-        <v>1.692403539</v>
+        <v>1.427259549</v>
       </c>
       <c r="M182" t="n">
-        <v>0.017361517</v>
+        <v>0.0172858608</v>
       </c>
     </row>
     <row r="183">
@@ -7570,25 +7570,25 @@
         <v>95</v>
       </c>
       <c r="G184" t="n">
-        <v>0.000776606</v>
+        <v>0.0008960563543</v>
       </c>
       <c r="H184" t="n">
-        <v>0.998398191</v>
+        <v>0.9979706128</v>
       </c>
       <c r="I184" t="n">
-        <v>50.86975184</v>
+        <v>47.47203793</v>
       </c>
       <c r="J184" t="n">
-        <v>0.328552297</v>
+        <v>0.2352792781</v>
       </c>
       <c r="K184" t="n">
-        <v>0.336501924</v>
+        <v>0.3840505824</v>
       </c>
       <c r="L184" t="n">
-        <v>0.485860491</v>
+        <v>0.5354910264</v>
       </c>
       <c r="M184" t="n">
-        <v>0.017474255</v>
+        <v>0.01740630779</v>
       </c>
     </row>
     <row r="185">
@@ -7646,25 +7646,25 @@
         <v>92</v>
       </c>
       <c r="G186" t="n">
-        <v>0.001481818</v>
+        <v>0.001649800079</v>
       </c>
       <c r="H186" t="n">
-        <v>0.999052642</v>
+        <v>0.9982468999</v>
       </c>
       <c r="I186" t="n">
-        <v>49.36266165</v>
+        <v>51.03013738</v>
       </c>
       <c r="J186" t="n">
-        <v>14.4210008</v>
+        <v>19.75685304</v>
       </c>
       <c r="K186" t="n">
-        <v>0.593606267</v>
+        <v>0.6153930042</v>
       </c>
       <c r="L186" t="n">
-        <v>1.173067077</v>
+        <v>1.171104075</v>
       </c>
       <c r="M186" t="n">
-        <v>0.017130761</v>
+        <v>0.01702138679</v>
       </c>
     </row>
     <row r="187">
@@ -7722,25 +7722,25 @@
         <v>92</v>
       </c>
       <c r="G188" t="n">
-        <v>0.000396267</v>
+        <v>0.0004941669981</v>
       </c>
       <c r="H188" t="n">
-        <v>0.998976795</v>
+        <v>0.996582247</v>
       </c>
       <c r="I188" t="n">
-        <v>58.93295166</v>
+        <v>60.59286224</v>
       </c>
       <c r="J188" t="n">
-        <v>12.2774006</v>
+        <v>31.24396363</v>
       </c>
       <c r="K188" t="n">
-        <v>0.23875548</v>
+        <v>0.2645548286</v>
       </c>
       <c r="L188" t="n">
-        <v>0.56197066</v>
+        <v>0.5893539287</v>
       </c>
       <c r="M188" t="n">
-        <v>0.017737721</v>
+        <v>0.01775102777</v>
       </c>
     </row>
     <row r="189">
@@ -7798,25 +7798,25 @@
         <v>95</v>
       </c>
       <c r="G190" t="n">
-        <v>0.001280225</v>
+        <v>0.00153746918</v>
       </c>
       <c r="H190" t="n">
-        <v>0.998833174</v>
+        <v>0.9983955637</v>
       </c>
       <c r="I190" t="n">
-        <v>47.53865145</v>
+        <v>48.6667972</v>
       </c>
       <c r="J190" t="n">
-        <v>4.674902758</v>
+        <v>19.75685304</v>
       </c>
       <c r="K190" t="n">
-        <v>0.603800166</v>
+        <v>0.5858252931</v>
       </c>
       <c r="L190" t="n">
-        <v>0.969789081</v>
+        <v>0.9463857716</v>
       </c>
       <c r="M190" t="n">
-        <v>0.017165356</v>
+        <v>0.01707299971</v>
       </c>
     </row>
     <row r="191">
@@ -7874,25 +7874,25 @@
         <v>95</v>
       </c>
       <c r="G192" t="n">
-        <v>0.000845547</v>
+        <v>0.001018217068</v>
       </c>
       <c r="H192" t="n">
-        <v>0.99874944</v>
+        <v>0.997214745</v>
       </c>
       <c r="I192" t="n">
-        <v>53.72619817</v>
+        <v>57.75443619</v>
       </c>
       <c r="J192" t="n">
-        <v>16.93886767</v>
+        <v>24.8451685</v>
       </c>
       <c r="K192" t="n">
-        <v>0.215343431</v>
+        <v>0.3107292407</v>
       </c>
       <c r="L192" t="n">
-        <v>0.488183342</v>
+        <v>0.5171701432</v>
       </c>
       <c r="M192" t="n">
-        <v>0.017330685</v>
+        <v>0.01724255824</v>
       </c>
     </row>
     <row r="193">
@@ -7950,25 +7950,25 @@
         <v>92</v>
       </c>
       <c r="G194" t="n">
-        <v>0.002321963</v>
+        <v>0.002371269874</v>
       </c>
       <c r="H194" t="n">
-        <v>0.998130672</v>
+        <v>0.9964977542</v>
       </c>
       <c r="I194" t="n">
-        <v>60.77933788</v>
+        <v>64.88962328</v>
       </c>
       <c r="J194" t="n">
-        <v>16.93886767</v>
+        <v>36.40118945</v>
       </c>
       <c r="K194" t="n">
-        <v>0.453695537</v>
+        <v>0.5062300147</v>
       </c>
       <c r="L194" t="n">
-        <v>0.619983092</v>
+        <v>0.7003591818</v>
       </c>
       <c r="M194" t="n">
-        <v>0.018228484</v>
+        <v>0.01830269105</v>
       </c>
     </row>
     <row r="195">
@@ -8026,25 +8026,25 @@
         <v>92</v>
       </c>
       <c r="G196" t="n">
-        <v>0.002451287</v>
+        <v>0.002608418627</v>
       </c>
       <c r="H196" t="n">
-        <v>0.995932428</v>
+        <v>0.9962122976</v>
       </c>
       <c r="I196" t="n">
-        <v>35.85415864</v>
+        <v>37.73982338</v>
       </c>
       <c r="J196" t="n">
-        <v>78.13212386</v>
+        <v>78.13809733</v>
       </c>
       <c r="K196" t="n">
-        <v>0.752312797</v>
+        <v>0.7440534086</v>
       </c>
       <c r="L196" t="n">
-        <v>0.900819911</v>
+        <v>0.8756408545</v>
       </c>
       <c r="M196" t="n">
-        <v>0.018160676</v>
+        <v>0.01826126676</v>
       </c>
     </row>
     <row r="197">
@@ -8102,25 +8102,25 @@
         <v>95</v>
       </c>
       <c r="G198" t="n">
-        <v>0.002453128</v>
+        <v>0.002461238008</v>
       </c>
       <c r="H198" t="n">
-        <v>0.999325468</v>
+        <v>0.9976585964</v>
       </c>
       <c r="I198" t="n">
-        <v>31.93174348</v>
+        <v>32.36781714</v>
       </c>
       <c r="J198" t="n">
-        <v>11.32822691</v>
+        <v>19.75685304</v>
       </c>
       <c r="K198" t="n">
-        <v>0.45591596</v>
+        <v>0.4693025626</v>
       </c>
       <c r="L198" t="n">
-        <v>0.808554753</v>
+        <v>0.8144845581</v>
       </c>
       <c r="M198" t="n">
-        <v>0.018445122</v>
+        <v>0.01850671007</v>
       </c>
     </row>
     <row r="199">
@@ -8178,25 +8178,25 @@
         <v>95</v>
       </c>
       <c r="G200" t="n">
-        <v>0.00174079</v>
+        <v>0.002026037738</v>
       </c>
       <c r="H200" t="n">
-        <v>0.998634085</v>
+        <v>0.9991265816</v>
       </c>
       <c r="I200" t="n">
-        <v>56.10034375</v>
+        <v>54.82280245</v>
       </c>
       <c r="J200" t="n">
-        <v>2.090873271</v>
+        <v>19.75685304</v>
       </c>
       <c r="K200" t="n">
-        <v>0.315675526</v>
+        <v>0.2905968305</v>
       </c>
       <c r="L200" t="n">
-        <v>0.489681454</v>
+        <v>0.4648210553</v>
       </c>
       <c r="M200" t="n">
-        <v>0.018433689</v>
+        <v>0.01855063605</v>
       </c>
     </row>
     <row r="201">
@@ -8252,25 +8252,25 @@
       <c r="E202"/>
       <c r="F202"/>
       <c r="G202" t="n">
-        <v>0.002497369</v>
+        <v>0.002497368973</v>
       </c>
       <c r="H202" t="n">
-        <v>0.996792344</v>
+        <v>0.9987851302</v>
       </c>
       <c r="I202" t="n">
-        <v>9.308210716</v>
+        <v>10.57108363</v>
       </c>
       <c r="J202" t="n">
-        <v>24.15583065</v>
+        <v>13.18123281</v>
       </c>
       <c r="K202" t="n">
-        <v>1.328369197</v>
+        <v>1.392910612</v>
       </c>
       <c r="L202" t="n">
-        <v>2.143404835</v>
+        <v>2.246877662</v>
       </c>
       <c r="M202" t="n">
-        <v>0.018656129</v>
+        <v>0.01865612926</v>
       </c>
     </row>
     <row r="203">
@@ -8324,25 +8324,25 @@
       <c r="E204"/>
       <c r="F204"/>
       <c r="G204" t="n">
-        <v>0.001207926</v>
+        <v>0.001207926056</v>
       </c>
       <c r="H204" t="n">
-        <v>0.998939031</v>
+        <v>0.9989063352</v>
       </c>
       <c r="I204" t="n">
-        <v>2.150905288</v>
+        <v>2.236939772</v>
       </c>
       <c r="J204" t="n">
-        <v>4.106716588</v>
+        <v>2.471172489</v>
       </c>
       <c r="K204" t="n">
-        <v>0.235830962</v>
+        <v>0.2792239687</v>
       </c>
       <c r="L204" t="n">
-        <v>0.725775631</v>
+        <v>0.7705203453</v>
       </c>
       <c r="M204" t="n">
-        <v>0.017151313</v>
+        <v>0.01715131292</v>
       </c>
     </row>
     <row r="205">
@@ -8396,25 +8396,25 @@
       <c r="E206"/>
       <c r="F206"/>
       <c r="G206" t="n">
-        <v>0.002741181</v>
+        <v>0.002741180913</v>
       </c>
       <c r="H206" t="n">
-        <v>0.998180066</v>
+        <v>0.9982507803</v>
       </c>
       <c r="I206" t="n">
-        <v>5.621358608</v>
+        <v>6.517426079</v>
       </c>
       <c r="J206" t="n">
-        <v>9.251128622</v>
+        <v>2.304672325</v>
       </c>
       <c r="K206" t="n">
-        <v>0.567820637</v>
+        <v>0.5974030287</v>
       </c>
       <c r="L206" t="n">
-        <v>1.920235313</v>
+        <v>2.243069181</v>
       </c>
       <c r="M206" t="n">
-        <v>0.018435108</v>
+        <v>0.01843510845</v>
       </c>
     </row>
     <row r="207">
@@ -8468,25 +8468,25 @@
       <c r="E208"/>
       <c r="F208"/>
       <c r="G208" t="n">
-        <v>0.001527964</v>
+        <v>0.001527963591</v>
       </c>
       <c r="H208" t="n">
-        <v>0.998477453</v>
+        <v>0.9992552423</v>
       </c>
       <c r="I208" t="n">
-        <v>2.80364994</v>
+        <v>2.863681175</v>
       </c>
       <c r="J208" t="n">
-        <v>4.760164956</v>
+        <v>4.96411459</v>
       </c>
       <c r="K208" t="n">
-        <v>0.238891331</v>
+        <v>0.2960700939</v>
       </c>
       <c r="L208" t="n">
-        <v>0.784581198</v>
+        <v>0.8130058735</v>
       </c>
       <c r="M208" t="n">
-        <v>0.017746369</v>
+        <v>0.01774636867</v>
       </c>
     </row>
     <row r="209">
@@ -8540,25 +8540,25 @@
       <c r="E210"/>
       <c r="F210"/>
       <c r="G210" t="n">
-        <v>0.001611834</v>
+        <v>0.00161183366</v>
       </c>
       <c r="H210" t="n">
-        <v>0.998738107</v>
+        <v>0.9990380229</v>
       </c>
       <c r="I210" t="n">
-        <v>8.80952165</v>
+        <v>12.03945469</v>
       </c>
       <c r="J210" t="n">
-        <v>3.542969895</v>
+        <v>0.8679504928</v>
       </c>
       <c r="K210" t="n">
-        <v>0.534082478</v>
+        <v>0.5622825894</v>
       </c>
       <c r="L210" t="n">
-        <v>1.333613117</v>
+        <v>1.548061886</v>
       </c>
       <c r="M210" t="n">
-        <v>0.018018255</v>
+        <v>0.01801825487</v>
       </c>
     </row>
     <row r="211">
@@ -8612,25 +8612,25 @@
       <c r="E212"/>
       <c r="F212"/>
       <c r="G212" t="n">
-        <v>0.002557239</v>
+        <v>0.00255723947</v>
       </c>
       <c r="H212" t="n">
-        <v>0.998851324</v>
+        <v>0.9990944353</v>
       </c>
       <c r="I212" t="n">
-        <v>2.54328739</v>
+        <v>2.776346432</v>
       </c>
       <c r="J212" t="n">
-        <v>1.57277818</v>
+        <v>0.7040659359</v>
       </c>
       <c r="K212" t="n">
-        <v>0.2612346</v>
+        <v>0.2441171874</v>
       </c>
       <c r="L212" t="n">
-        <v>0.789202721</v>
+        <v>0.8005582883</v>
       </c>
       <c r="M212" t="n">
-        <v>0.017446715</v>
+        <v>0.01744671518</v>
       </c>
     </row>
     <row r="213">
@@ -8684,22 +8684,22 @@
       <c r="E214"/>
       <c r="F214"/>
       <c r="G214" t="n">
-        <v>0.00624885</v>
+        <v>0.006248850204</v>
       </c>
       <c r="H214" t="n">
-        <v>0.998842613</v>
+        <v>0.9981115521</v>
       </c>
       <c r="I214" t="n">
-        <v>1.607141904</v>
+        <v>1.769674314</v>
       </c>
       <c r="J214" t="n">
-        <v>1.460843997</v>
+        <v>0.4029603757</v>
       </c>
       <c r="K214" t="n">
-        <v>0.469801094</v>
+        <v>0.4946464452</v>
       </c>
       <c r="L214" t="n">
-        <v>1.316650475</v>
+        <v>1.344782923</v>
       </c>
       <c r="M214" t="n">
         <v>0.020194359</v>
@@ -8756,25 +8756,25 @@
       <c r="E216"/>
       <c r="F216"/>
       <c r="G216" t="n">
-        <v>0.003363863</v>
+        <v>0.003363863486</v>
       </c>
       <c r="H216" t="n">
-        <v>0.998112053</v>
+        <v>0.9990944618</v>
       </c>
       <c r="I216" t="n">
-        <v>6.511572224</v>
+        <v>7.391159844</v>
       </c>
       <c r="J216" t="n">
-        <v>24.15583065</v>
+        <v>8.089075974</v>
       </c>
       <c r="K216" t="n">
-        <v>1.575018208</v>
+        <v>1.594739528</v>
       </c>
       <c r="L216" t="n">
-        <v>2.830659827</v>
+        <v>2.713974409</v>
       </c>
       <c r="M216" t="n">
-        <v>0.018641153</v>
+        <v>0.0186411527</v>
       </c>
     </row>
     <row r="217">
@@ -8828,25 +8828,25 @@
       <c r="E218"/>
       <c r="F218"/>
       <c r="G218" t="n">
-        <v>0.002936614</v>
+        <v>0.002936613867</v>
       </c>
       <c r="H218" t="n">
-        <v>0.997689352</v>
+        <v>0.9971469768</v>
       </c>
       <c r="I218" t="n">
-        <v>2.525680929</v>
+        <v>2.979608517</v>
       </c>
       <c r="J218" t="n">
-        <v>0.248357109</v>
+        <v>0.2005966173</v>
       </c>
       <c r="K218" t="n">
-        <v>0.415814283</v>
+        <v>0.4764487463</v>
       </c>
       <c r="L218" t="n">
-        <v>0.784701051</v>
+        <v>0.9200220785</v>
       </c>
       <c r="M218" t="n">
-        <v>0.018790941</v>
+        <v>0.01879094063</v>
       </c>
     </row>
     <row r="219">
@@ -8900,25 +8900,25 @@
       <c r="E220"/>
       <c r="F220"/>
       <c r="G220" t="n">
-        <v>0.000398862</v>
+        <v>0.0003988616117</v>
       </c>
       <c r="H220" t="n">
-        <v>0.998277354</v>
+        <v>0.9992354141</v>
       </c>
       <c r="I220" t="n">
-        <v>9.356764506</v>
+        <v>11.4752327</v>
       </c>
       <c r="J220" t="n">
-        <v>14.40709866</v>
+        <v>1.869509022</v>
       </c>
       <c r="K220" t="n">
-        <v>0.747548129</v>
+        <v>0.7906935246</v>
       </c>
       <c r="L220" t="n">
-        <v>1.48117707</v>
+        <v>1.465227048</v>
       </c>
       <c r="M220" t="n">
-        <v>0.017648197</v>
+        <v>0.01764819729</v>
       </c>
     </row>
     <row r="221">
@@ -8972,25 +8972,25 @@
       <c r="E222"/>
       <c r="F222"/>
       <c r="G222" t="n">
-        <v>0.002015098</v>
+        <v>0.002015098422</v>
       </c>
       <c r="H222" t="n">
-        <v>0.998759483</v>
+        <v>0.9986299366</v>
       </c>
       <c r="I222" t="n">
-        <v>3.547817429</v>
+        <v>4.025461282</v>
       </c>
       <c r="J222" t="n">
-        <v>2.27908865</v>
+        <v>0.7053243869</v>
       </c>
       <c r="K222" t="n">
-        <v>0.472793936</v>
+        <v>0.5745940106</v>
       </c>
       <c r="L222" t="n">
-        <v>0.830423955</v>
+        <v>0.9623382569</v>
       </c>
       <c r="M222" t="n">
-        <v>0.017776682</v>
+        <v>0.01777668228</v>
       </c>
     </row>
     <row r="223">
@@ -9044,25 +9044,25 @@
       <c r="E224"/>
       <c r="F224"/>
       <c r="G224" t="n">
-        <v>0.001374148</v>
+        <v>0.001374148085</v>
       </c>
       <c r="H224" t="n">
-        <v>0.998747438</v>
+        <v>0.9992220177</v>
       </c>
       <c r="I224" t="n">
-        <v>3.133722524</v>
+        <v>3.370453436</v>
       </c>
       <c r="J224" t="n">
-        <v>1.575589372</v>
+        <v>0.869501872</v>
       </c>
       <c r="K224" t="n">
-        <v>0.313128335</v>
+        <v>0.3665928083</v>
       </c>
       <c r="L224" t="n">
-        <v>0.658570814</v>
+        <v>0.6931811469</v>
       </c>
       <c r="M224" t="n">
-        <v>0.017312785</v>
+        <v>0.01731278487</v>
       </c>
     </row>
     <row r="225">
@@ -9116,25 +9116,25 @@
       <c r="E226"/>
       <c r="F226"/>
       <c r="G226" t="n">
-        <v>0.001598971</v>
+        <v>0.001598970816</v>
       </c>
       <c r="H226" t="n">
-        <v>0.998867894</v>
+        <v>0.998959671</v>
       </c>
       <c r="I226" t="n">
-        <v>4.603142435</v>
+        <v>5.623537426</v>
       </c>
       <c r="J226" t="n">
-        <v>1.359301425</v>
+        <v>0.4328443807</v>
       </c>
       <c r="K226" t="n">
-        <v>0.341743949</v>
+        <v>0.4132042531</v>
       </c>
       <c r="L226" t="n">
-        <v>0.843399527</v>
+        <v>0.9724676261</v>
       </c>
       <c r="M226" t="n">
-        <v>0.017588785</v>
+        <v>0.01758878535</v>
       </c>
     </row>
     <row r="227">
@@ -9188,25 +9188,25 @@
       <c r="E228"/>
       <c r="F228"/>
       <c r="G228" t="n">
-        <v>0.002319588</v>
+        <v>0.002319587693</v>
       </c>
       <c r="H228" t="n">
-        <v>0.998410605</v>
+        <v>0.9980742265</v>
       </c>
       <c r="I228" t="n">
-        <v>5.349714799</v>
+        <v>6.294519503</v>
       </c>
       <c r="J228" t="n">
-        <v>1.826292405</v>
+        <v>0.6134810504</v>
       </c>
       <c r="K228" t="n">
-        <v>0.416044569</v>
+        <v>0.4898209223</v>
       </c>
       <c r="L228" t="n">
-        <v>0.965038183</v>
+        <v>1.166893765</v>
       </c>
       <c r="M228" t="n">
-        <v>0.017728293</v>
+        <v>0.01772829343</v>
       </c>
     </row>
     <row r="229">
@@ -9260,25 +9260,25 @@
       <c r="E230"/>
       <c r="F230"/>
       <c r="G230" t="n">
-        <v>0.004003784</v>
+        <v>0.004003783605</v>
       </c>
       <c r="H230" t="n">
-        <v>0.999362922</v>
+        <v>0.9983478885</v>
       </c>
       <c r="I230" t="n">
-        <v>2.38253027</v>
+        <v>2.566894033</v>
       </c>
       <c r="J230" t="n">
-        <v>0.44911881</v>
+        <v>0.2848187271</v>
       </c>
       <c r="K230" t="n">
-        <v>0.219242261</v>
+        <v>0.2533298612</v>
       </c>
       <c r="L230" t="n">
-        <v>0.691678266</v>
+        <v>0.7570702786</v>
       </c>
       <c r="M230" t="n">
-        <v>0.01613179</v>
+        <v>0.01613178951</v>
       </c>
     </row>
     <row r="231">
@@ -9332,25 +9332,25 @@
       <c r="E232"/>
       <c r="F232"/>
       <c r="G232" t="n">
-        <v>0.002164642</v>
+        <v>0.002164641667</v>
       </c>
       <c r="H232" t="n">
-        <v>0.998975179</v>
+        <v>0.9972995369</v>
       </c>
       <c r="I232" t="n">
-        <v>4.402523859</v>
+        <v>5.366511868</v>
       </c>
       <c r="J232" t="n">
-        <v>1.696315685</v>
+        <v>0.5721465437</v>
       </c>
       <c r="K232" t="n">
-        <v>0.497258155</v>
+        <v>0.5831522012</v>
       </c>
       <c r="L232" t="n">
-        <v>0.964603357</v>
+        <v>1.128906332</v>
       </c>
       <c r="M232" t="n">
-        <v>0.018456007</v>
+        <v>0.0184560074</v>
       </c>
     </row>
     <row r="233">
@@ -9404,25 +9404,25 @@
       <c r="E234"/>
       <c r="F234"/>
       <c r="G234" t="n">
-        <v>0.00196486</v>
+        <v>0.001964860107</v>
       </c>
       <c r="H234" t="n">
-        <v>0.997168268</v>
+        <v>0.9972427458</v>
       </c>
       <c r="I234" t="n">
-        <v>1.993351348</v>
+        <v>2.255922934</v>
       </c>
       <c r="J234" t="n">
-        <v>4.114056954</v>
+        <v>3.762199924</v>
       </c>
       <c r="K234" t="n">
-        <v>0.435024576</v>
+        <v>0.5700520843</v>
       </c>
       <c r="L234" t="n">
-        <v>1.023725068</v>
+        <v>1.161245412</v>
       </c>
       <c r="M234" t="n">
-        <v>0.017603595</v>
+        <v>0.01760359512</v>
       </c>
     </row>
     <row r="235">
@@ -9476,25 +9476,25 @@
       <c r="E236"/>
       <c r="F236"/>
       <c r="G236" t="n">
-        <v>0.008242305</v>
+        <v>0.008242304939</v>
       </c>
       <c r="H236" t="n">
-        <v>0.998548411</v>
+        <v>0.9984379394</v>
       </c>
       <c r="I236" t="n">
-        <v>2.615928344</v>
+        <v>3.196936703</v>
       </c>
       <c r="J236" t="n">
-        <v>3.296699742</v>
+        <v>1.416862277</v>
       </c>
       <c r="K236" t="n">
-        <v>0.321646687</v>
+        <v>0.3639931278</v>
       </c>
       <c r="L236" t="n">
-        <v>0.799773377</v>
+        <v>1.020091096</v>
       </c>
       <c r="M236" t="n">
-        <v>0.018094707</v>
+        <v>0.01809470653</v>
       </c>
     </row>
     <row r="237">
@@ -9548,25 +9548,25 @@
       <c r="E238"/>
       <c r="F238"/>
       <c r="G238" t="n">
-        <v>0.001314596</v>
+        <v>0.001314585174</v>
       </c>
       <c r="H238" t="n">
-        <v>0.999181485</v>
+        <v>0.9980580549</v>
       </c>
       <c r="I238" t="n">
-        <v>2.37860258</v>
+        <v>2.583375946</v>
       </c>
       <c r="J238" t="n">
-        <v>1.011722088</v>
+        <v>0.3053953463</v>
       </c>
       <c r="K238" t="n">
-        <v>0.522489478</v>
+        <v>0.5475636663</v>
       </c>
       <c r="L238" t="n">
-        <v>0.944067774</v>
+        <v>1.085502078</v>
       </c>
       <c r="M238" t="n">
-        <v>0.018021391</v>
+        <v>0.0180213882</v>
       </c>
     </row>
     <row r="239">
@@ -9620,25 +9620,25 @@
       <c r="E240"/>
       <c r="F240"/>
       <c r="G240" t="n">
-        <v>0.005221996</v>
+        <v>0.005221995624</v>
       </c>
       <c r="H240" t="n">
-        <v>0.99832448</v>
+        <v>0.998383955</v>
       </c>
       <c r="I240" t="n">
-        <v>2.867665758</v>
+        <v>3.679019886</v>
       </c>
       <c r="J240" t="n">
-        <v>0.41715515</v>
+        <v>0.3274585155</v>
       </c>
       <c r="K240" t="n">
-        <v>0.476099368</v>
+        <v>0.4990315413</v>
       </c>
       <c r="L240" t="n">
-        <v>1.603440466</v>
+        <v>2.067776774</v>
       </c>
       <c r="M240" t="n">
-        <v>0.018762949</v>
+        <v>0.01876294872</v>
       </c>
     </row>
     <row r="241">
@@ -9692,25 +9692,25 @@
       <c r="E242"/>
       <c r="F242"/>
       <c r="G242" t="n">
-        <v>0.003165475</v>
+        <v>0.003165474784</v>
       </c>
       <c r="H242" t="n">
-        <v>0.998522498</v>
+        <v>0.9989085143</v>
       </c>
       <c r="I242" t="n">
-        <v>2.307964304</v>
+        <v>2.481635398</v>
       </c>
       <c r="J242" t="n">
-        <v>2.637016951</v>
+        <v>1.626072174</v>
       </c>
       <c r="K242" t="n">
-        <v>0.537598516</v>
+        <v>0.6354807573</v>
       </c>
       <c r="L242" t="n">
-        <v>0.945207842</v>
+        <v>0.9795674545</v>
       </c>
       <c r="M242" t="n">
-        <v>0.016852209</v>
+        <v>0.01685220944</v>
       </c>
     </row>
     <row r="243">
@@ -9764,25 +9764,25 @@
       <c r="E244"/>
       <c r="F244"/>
       <c r="G244" t="n">
-        <v>0.002151629</v>
+        <v>0.002151629239</v>
       </c>
       <c r="H244" t="n">
-        <v>0.999091822</v>
+        <v>0.9928499718</v>
       </c>
       <c r="I244" t="n">
-        <v>5.645974739</v>
+        <v>7.543740545</v>
       </c>
       <c r="J244" t="n">
-        <v>0.184851107</v>
+        <v>0.02307881568</v>
       </c>
       <c r="K244" t="n">
-        <v>0.19885573</v>
+        <v>0.2084701882</v>
       </c>
       <c r="L244" t="n">
-        <v>0.419978432</v>
+        <v>0.6504150776</v>
       </c>
       <c r="M244" t="n">
-        <v>0.017720722</v>
+        <v>0.01772072222</v>
       </c>
     </row>
     <row r="245">
@@ -9836,25 +9836,25 @@
       <c r="E246"/>
       <c r="F246"/>
       <c r="G246" t="n">
-        <v>0.001145127</v>
+        <v>0.001145127179</v>
       </c>
       <c r="H246" t="n">
-        <v>0.996254709</v>
+        <v>0.9972241189</v>
       </c>
       <c r="I246" t="n">
-        <v>2.567221318</v>
+        <v>3.345962699</v>
       </c>
       <c r="J246" t="n">
-        <v>0.248357109</v>
+        <v>0.02152383454</v>
       </c>
       <c r="K246" t="n">
-        <v>0.541497278</v>
+        <v>0.8297868743</v>
       </c>
       <c r="L246" t="n">
-        <v>1.225121517</v>
+        <v>1.476394998</v>
       </c>
       <c r="M246" t="n">
-        <v>0.018090906</v>
+        <v>0.01809090569</v>
       </c>
     </row>
     <row r="247">
@@ -9908,25 +9908,25 @@
       <c r="E248"/>
       <c r="F248"/>
       <c r="G248" t="n">
-        <v>0.001605707</v>
+        <v>0.001605707112</v>
       </c>
       <c r="H248" t="n">
-        <v>0.999157129</v>
+        <v>0.9983954072</v>
       </c>
       <c r="I248" t="n">
-        <v>4.521951677</v>
+        <v>5.378756986</v>
       </c>
       <c r="J248" t="n">
-        <v>1.087299779</v>
+        <v>0.4967569638</v>
       </c>
       <c r="K248" t="n">
-        <v>0.477867064</v>
+        <v>0.4421616629</v>
       </c>
       <c r="L248" t="n">
-        <v>1.136150895</v>
+        <v>1.202305523</v>
       </c>
       <c r="M248" t="n">
-        <v>0.017951478</v>
+        <v>0.01795147839</v>
       </c>
     </row>
     <row r="249">
@@ -9980,25 +9980,25 @@
       <c r="E250"/>
       <c r="F250"/>
       <c r="G250" t="n">
-        <v>0.004730907</v>
+        <v>0.004730906524</v>
       </c>
       <c r="H250" t="n">
-        <v>0.998441338</v>
+        <v>0.9985936718</v>
       </c>
       <c r="I250" t="n">
-        <v>0.840671315</v>
+        <v>0.8373208818</v>
       </c>
       <c r="J250" t="n">
-        <v>4.106716588</v>
+        <v>6.119605403</v>
       </c>
       <c r="K250" t="n">
-        <v>0.236181261</v>
+        <v>0.2372713805</v>
       </c>
       <c r="L250" t="n">
-        <v>0.645263226</v>
+        <v>0.6548498712</v>
       </c>
       <c r="M250" t="n">
-        <v>0.017024155</v>
+        <v>0.01702415473</v>
       </c>
     </row>
     <row r="251">
@@ -10052,25 +10052,25 @@
       <c r="E252"/>
       <c r="F252"/>
       <c r="G252" t="n">
-        <v>0.005048873</v>
+        <v>0.005048872863</v>
       </c>
       <c r="H252" t="n">
-        <v>0.998607157</v>
+        <v>0.997674166</v>
       </c>
       <c r="I252" t="n">
-        <v>2.860816577</v>
+        <v>3.132390077</v>
       </c>
       <c r="J252" t="n">
-        <v>0.267386965</v>
+        <v>0.02307881568</v>
       </c>
       <c r="K252" t="n">
-        <v>0.394743189</v>
+        <v>0.4032856382</v>
       </c>
       <c r="L252" t="n">
-        <v>0.959679217</v>
+        <v>1.139738048</v>
       </c>
       <c r="M252" t="n">
-        <v>0.019839747</v>
+        <v>0.01983974679</v>
       </c>
     </row>
     <row r="253">
@@ -10124,25 +10124,25 @@
       <c r="E254"/>
       <c r="F254"/>
       <c r="G254" t="n">
-        <v>0.006600089</v>
+        <v>0.006600089152</v>
       </c>
       <c r="H254" t="n">
-        <v>0.997452031</v>
+        <v>0.9972935424</v>
       </c>
       <c r="I254" t="n">
-        <v>1.673980018</v>
+        <v>1.803013841</v>
       </c>
       <c r="J254" t="n">
-        <v>0.248357109</v>
+        <v>0.2005966173</v>
       </c>
       <c r="K254" t="n">
-        <v>0.423831716</v>
+        <v>0.5206435615</v>
       </c>
       <c r="L254" t="n">
-        <v>0.886896189</v>
+        <v>1.056125247</v>
       </c>
       <c r="M254" t="n">
-        <v>0.01917068</v>
+        <v>0.01917068037</v>
       </c>
     </row>
     <row r="255">
@@ -10196,25 +10196,25 @@
       <c r="E256"/>
       <c r="F256"/>
       <c r="G256" t="n">
-        <v>0.007925134</v>
+        <v>0.007925134399</v>
       </c>
       <c r="H256" t="n">
-        <v>0.997776133</v>
+        <v>0.9986430277</v>
       </c>
       <c r="I256" t="n">
-        <v>1.277976802</v>
+        <v>1.283007923</v>
       </c>
       <c r="J256" t="n">
-        <v>30.14483296</v>
+        <v>30.44265429</v>
       </c>
       <c r="K256" t="n">
-        <v>0.318137304</v>
+        <v>0.3343471435</v>
       </c>
       <c r="L256" t="n">
-        <v>0.569794215</v>
+        <v>0.57369698</v>
       </c>
       <c r="M256" t="n">
-        <v>0.020010196</v>
+        <v>0.02001019556</v>
       </c>
     </row>
     <row r="257">
@@ -10268,25 +10268,25 @@
       <c r="E258"/>
       <c r="F258"/>
       <c r="G258" t="n">
-        <v>0.005798405</v>
+        <v>0.005798404857</v>
       </c>
       <c r="H258" t="n">
-        <v>0.99936771</v>
+        <v>0.9993623986</v>
       </c>
       <c r="I258" t="n">
-        <v>0.792990213</v>
+        <v>0.7917519407</v>
       </c>
       <c r="J258" t="n">
-        <v>0.333680738</v>
+        <v>0.3504891638</v>
       </c>
       <c r="K258" t="n">
-        <v>0.255755951</v>
+        <v>0.2542400942</v>
       </c>
       <c r="L258" t="n">
-        <v>0.636459611</v>
+        <v>0.6381518996</v>
       </c>
       <c r="M258" t="n">
-        <v>0.017902139</v>
+        <v>0.01790213881</v>
       </c>
     </row>
     <row r="259">
@@ -10340,25 +10340,25 @@
       <c r="E260"/>
       <c r="F260"/>
       <c r="G260" t="n">
-        <v>0.001323687</v>
+        <v>0.001323686662</v>
       </c>
       <c r="H260" t="n">
-        <v>0.996443674</v>
+        <v>0.9979554509</v>
       </c>
       <c r="I260" t="n">
-        <v>2.354877312</v>
+        <v>2.856355289</v>
       </c>
       <c r="J260" t="n">
-        <v>577.7743903</v>
+        <v>0.2651545599</v>
       </c>
       <c r="K260" t="n">
-        <v>0.439036876</v>
+        <v>1.150174306</v>
       </c>
       <c r="L260" t="n">
-        <v>0.553179806</v>
+        <v>1.787192949</v>
       </c>
       <c r="M260" t="n">
-        <v>0.018264309</v>
+        <v>0.01826430911</v>
       </c>
     </row>
     <row r="261">
@@ -10412,25 +10412,25 @@
       <c r="E262"/>
       <c r="F262"/>
       <c r="G262" t="n">
-        <v>0.004515766</v>
+        <v>0.00451576597</v>
       </c>
       <c r="H262" t="n">
-        <v>0.998735788</v>
+        <v>0.997154982</v>
       </c>
       <c r="I262" t="n">
-        <v>1.044714249</v>
+        <v>1.086428135</v>
       </c>
       <c r="J262" t="n">
-        <v>0.44911881</v>
+        <v>0.3764818433</v>
       </c>
       <c r="K262" t="n">
-        <v>0.321858616</v>
+        <v>0.3754673647</v>
       </c>
       <c r="L262" t="n">
-        <v>0.558063788</v>
+        <v>0.6162093871</v>
       </c>
       <c r="M262" t="n">
-        <v>0.017185191</v>
+        <v>0.0171851908</v>
       </c>
     </row>
     <row r="263">
@@ -10484,25 +10484,25 @@
       <c r="E264"/>
       <c r="F264"/>
       <c r="G264" t="n">
-        <v>0.001674514</v>
+        <v>0.001674513564</v>
       </c>
       <c r="H264" t="n">
-        <v>0.999283158</v>
+        <v>0.9993224798</v>
       </c>
       <c r="I264" t="n">
-        <v>2.77797854</v>
+        <v>2.80639215</v>
       </c>
       <c r="J264" t="n">
-        <v>1.826292405</v>
+        <v>1.872850592</v>
       </c>
       <c r="K264" t="n">
-        <v>0.150247611</v>
+        <v>0.1553091062</v>
       </c>
       <c r="L264" t="n">
-        <v>0.396202131</v>
+        <v>0.4246988587</v>
       </c>
       <c r="M264" t="n">
-        <v>0.016979689</v>
+        <v>0.01697968866</v>
       </c>
     </row>
     <row r="265">
@@ -10556,25 +10556,25 @@
       <c r="E266"/>
       <c r="F266"/>
       <c r="G266" t="n">
-        <v>0.007887921</v>
+        <v>0.007887921169</v>
       </c>
       <c r="H266" t="n">
-        <v>0.999014544</v>
+        <v>0.9989535673</v>
       </c>
       <c r="I266" t="n">
-        <v>0.834382949</v>
+        <v>0.836322376</v>
       </c>
       <c r="J266" t="n">
-        <v>2.844147555</v>
+        <v>2.475589476</v>
       </c>
       <c r="K266" t="n">
-        <v>0.23742786</v>
+        <v>0.2415390813</v>
       </c>
       <c r="L266" t="n">
-        <v>0.443767838</v>
+        <v>0.4452693998</v>
       </c>
       <c r="M266" t="n">
-        <v>0.017661177</v>
+        <v>0.01766117694</v>
       </c>
     </row>
     <row r="267">
@@ -10628,25 +10628,25 @@
       <c r="E268"/>
       <c r="F268"/>
       <c r="G268" t="n">
-        <v>0.006700542</v>
+        <v>0.006700542038</v>
       </c>
       <c r="H268" t="n">
-        <v>0.999002586</v>
+        <v>0.9988999039</v>
       </c>
       <c r="I268" t="n">
-        <v>0.80637089</v>
+        <v>0.8045920272</v>
       </c>
       <c r="J268" t="n">
-        <v>1.463455117</v>
+        <v>1.519222947</v>
       </c>
       <c r="K268" t="n">
-        <v>0.219749375</v>
+        <v>0.2226955581</v>
       </c>
       <c r="L268" t="n">
-        <v>0.362871045</v>
+        <v>0.362854394</v>
       </c>
       <c r="M268" t="n">
-        <v>0.016852429</v>
+        <v>0.01685242918</v>
       </c>
     </row>
     <row r="269">
@@ -10700,25 +10700,25 @@
       <c r="E270"/>
       <c r="F270"/>
       <c r="G270" t="n">
-        <v>0.003714559</v>
+        <v>0.003714558856</v>
       </c>
       <c r="H270" t="n">
-        <v>0.997350928</v>
+        <v>0.9978852651</v>
       </c>
       <c r="I270" t="n">
-        <v>1.259813993</v>
+        <v>1.268869278</v>
       </c>
       <c r="J270" t="n">
-        <v>0.214647035</v>
+        <v>0.2310398638</v>
       </c>
       <c r="K270" t="n">
-        <v>0.216082849</v>
+        <v>0.2295236835</v>
       </c>
       <c r="L270" t="n">
-        <v>0.466835617</v>
+        <v>0.4898670178</v>
       </c>
       <c r="M270" t="n">
-        <v>0.017648244</v>
+        <v>0.01764824366</v>
       </c>
     </row>
     <row r="271">
@@ -10772,25 +10772,25 @@
       <c r="E272"/>
       <c r="F272"/>
       <c r="G272" t="n">
-        <v>0.005346324</v>
+        <v>0.005346323534</v>
       </c>
       <c r="H272" t="n">
-        <v>0.998677472</v>
+        <v>0.997134209</v>
       </c>
       <c r="I272" t="n">
-        <v>6.43937731</v>
+        <v>8.282732173</v>
       </c>
       <c r="J272" t="n">
-        <v>0.248801024</v>
+        <v>0.02156230635</v>
       </c>
       <c r="K272" t="n">
-        <v>0.379248519</v>
+        <v>0.4275118357</v>
       </c>
       <c r="L272" t="n">
-        <v>0.607296621</v>
+        <v>0.7838887177</v>
       </c>
       <c r="M272" t="n">
-        <v>0.018765024</v>
+        <v>0.01876502383</v>
       </c>
     </row>
     <row r="273">
@@ -10844,25 +10844,25 @@
       <c r="E274"/>
       <c r="F274"/>
       <c r="G274" t="n">
-        <v>0.005882299</v>
+        <v>0.005882298625</v>
       </c>
       <c r="H274" t="n">
-        <v>0.997522878</v>
+        <v>0.9972647387</v>
       </c>
       <c r="I274" t="n">
-        <v>1.590235962</v>
+        <v>1.777125791</v>
       </c>
       <c r="J274" t="n">
-        <v>0.288389493</v>
+        <v>0.2154730932</v>
       </c>
       <c r="K274" t="n">
-        <v>0.914044976</v>
+        <v>1.190505461</v>
       </c>
       <c r="L274" t="n">
-        <v>1.080132769</v>
+        <v>1.427259757</v>
       </c>
       <c r="M274" t="n">
-        <v>0.018581198</v>
+        <v>0.0185811976</v>
       </c>
     </row>
     <row r="275">
@@ -10916,25 +10916,25 @@
       <c r="E276"/>
       <c r="F276"/>
       <c r="G276" t="n">
-        <v>0.00033554</v>
+        <v>0.0003355399204</v>
       </c>
       <c r="H276" t="n">
-        <v>0.995283554</v>
+        <v>0.9966382578</v>
       </c>
       <c r="I276" t="n">
-        <v>1.678392222</v>
+        <v>1.772005873</v>
       </c>
       <c r="J276" t="n">
-        <v>20.87710489</v>
+        <v>4.325433284</v>
       </c>
       <c r="K276" t="n">
-        <v>0.857761907</v>
+        <v>0.8329872936</v>
       </c>
       <c r="L276" t="n">
-        <v>1.179110486</v>
+        <v>1.250906707</v>
       </c>
       <c r="M276" t="n">
-        <v>0.017697052</v>
+        <v>0.01769705167</v>
       </c>
     </row>
     <row r="277">
@@ -10988,25 +10988,25 @@
       <c r="E278"/>
       <c r="F278"/>
       <c r="G278" t="n">
-        <v>0.0034027</v>
+        <v>0.003402700285</v>
       </c>
       <c r="H278" t="n">
-        <v>0.997551501</v>
+        <v>0.998227809</v>
       </c>
       <c r="I278" t="n">
-        <v>2.312486407</v>
+        <v>2.747241046</v>
       </c>
       <c r="J278" t="n">
-        <v>0.93971811</v>
+        <v>0.4641150562</v>
       </c>
       <c r="K278" t="n">
-        <v>0.754058708</v>
+        <v>0.6891430375</v>
       </c>
       <c r="L278" t="n">
-        <v>1.61062611</v>
+        <v>1.642895783</v>
       </c>
       <c r="M278" t="n">
-        <v>0.018977718</v>
+        <v>0.01897771794</v>
       </c>
     </row>
     <row r="279">
@@ -11060,25 +11060,25 @@
       <c r="E280"/>
       <c r="F280"/>
       <c r="G280" t="n">
-        <v>0.001219625</v>
+        <v>0.001219624955</v>
       </c>
       <c r="H280" t="n">
-        <v>0.998831146</v>
+        <v>0.9991351107</v>
       </c>
       <c r="I280" t="n">
-        <v>1.414700698</v>
+        <v>1.437607172</v>
       </c>
       <c r="J280" t="n">
-        <v>1.696315685</v>
+        <v>1.321398361</v>
       </c>
       <c r="K280" t="n">
-        <v>0.370551997</v>
+        <v>0.3912929804</v>
       </c>
       <c r="L280" t="n">
-        <v>0.78502233</v>
+        <v>0.8204300259</v>
       </c>
       <c r="M280" t="n">
-        <v>0.017497969</v>
+        <v>0.01749796943</v>
       </c>
     </row>
     <row r="281">

</xml_diff>

<commit_message>
Finalizing scripts 1-2, continuing script 3
SSFA_1_Import.Rmd:
- load packages from character vector in order to...
- ... cite used packages in HTML/MD report
- renaming of NMP categories

SSFA_2_ Summary-stats.Rmd:
- load packages from character vector in order to...
- ... cite used packages in HTML/MD report
- additionally group by NMP_cat
- exclude surfaces with NMP > 20%

SSFA_3_Plots.Rmd:
- load packages from character vector in order to...
- ... cite used packages in HTML/MD report
- exclude surfaces with NMP > 20%
- shapes defined by NMP_cat
- unresolved issue with position_jitterdodge() when shape aesthetics are used only for geom_point() and not for geom_boxplot()
</commit_message>
<xml_diff>
--- a/R_analysis/derived_data/SSFA_all_data.xlsx
+++ b/R_analysis/derived_data/SSFA_all_data.xlsx
@@ -72,7 +72,7 @@
     <t xml:space="preserve">Dry lucerne</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;5%</t>
+    <t xml:space="preserve">0-5%</t>
   </si>
   <si>
     <t xml:space="preserve">Toothfrax</t>
@@ -342,7 +342,7 @@
     <t xml:space="preserve">Control</t>
   </si>
   <si>
-    <t xml:space="preserve">&gt;20%</t>
+    <t xml:space="preserve">20-100%</t>
   </si>
   <si>
     <t xml:space="preserve">FLT3-8_LSM_50x-0.95_20190321_Area2_Topo</t>

</xml_diff>